<commit_message>
Aanpassing configuratie van Bij12 aan Geonovum
Bij12 volgt nu "integraal" de Geonovum configuratie.

Dit is een minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BIJ12/props/BIJ12.xlsx
+++ b/src/main/resources/input/BIJ12/props/BIJ12.xlsx
@@ -852,9 +852,6 @@
     <t>SIM: opleveren</t>
   </si>
   <si>
-    <t>SIM</t>
-  </si>
-  <si>
     <t>SIM: minimum</t>
   </si>
   <si>
@@ -966,7 +963,10 @@
     <t>BIJ12_GEOSTANDAARDEN</t>
   </si>
   <si>
-    <t>BIJ12SIM</t>
+    <t>BIJ12CM</t>
+  </si>
+  <si>
+    <t>CM</t>
   </si>
 </sst>
 </file>
@@ -1543,13 +1543,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M139"/>
+  <dimension ref="A1:L139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F82" sqref="F82"/>
+      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1605,10 +1605,10 @@
       <c r="F2" s="3"/>
       <c r="G2" s="19"/>
       <c r="H2" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>277</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>274</v>
@@ -1954,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G18" s="20"/>
       <c r="K18" s="20"/>
@@ -1997,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G20" s="20"/>
       <c r="K20" s="20"/>
@@ -2020,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G21" s="20"/>
       <c r="K21" s="20"/>
@@ -2158,13 +2158,13 @@
     </row>
     <row r="27" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="46" t="s">
         <v>299</v>
-      </c>
-      <c r="B27" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>300</v>
       </c>
       <c r="D27" s="46" t="b">
         <v>0</v>
@@ -2285,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G31" s="27"/>
       <c r="H31" s="31"/>
@@ -2416,13 +2416,13 @@
     </row>
     <row r="37" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="38" t="s">
         <v>278</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>279</v>
       </c>
       <c r="D37" s="38" t="b">
         <v>0</v>
@@ -2438,13 +2438,13 @@
     </row>
     <row r="38" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="48" t="s">
+        <v>304</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="48" t="s">
         <v>305</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="48" t="s">
-        <v>306</v>
       </c>
       <c r="D38" s="48" t="b">
         <v>0</v>
@@ -2544,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G42" s="27"/>
       <c r="H42" s="35"/>
@@ -2735,8 +2735,8 @@
       <c r="E51" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>313</v>
+      <c r="F51" s="50" t="s">
+        <v>312</v>
       </c>
       <c r="G51" s="21"/>
       <c r="H51" s="43"/>
@@ -2885,13 +2885,13 @@
     </row>
     <row r="58" spans="1:12" s="47" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="47" t="s">
+        <v>300</v>
+      </c>
+      <c r="B58" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="47" t="s">
         <v>301</v>
-      </c>
-      <c r="B58" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="47" t="s">
-        <v>302</v>
       </c>
       <c r="D58" s="47" t="b">
         <v>0</v>
@@ -2914,13 +2914,13 @@
     </row>
     <row r="59" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D59" s="16" t="b">
         <v>0</v>
@@ -2938,35 +2938,35 @@
     </row>
     <row r="60" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>289</v>
       </c>
       <c r="G60" s="27"/>
       <c r="K60" s="27"/>
     </row>
     <row r="61" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D61" s="7" t="b">
         <v>0</v>
@@ -3050,7 +3050,7 @@
       <c r="K64" s="20"/>
       <c r="L64"/>
     </row>
-    <row r="65" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -3073,7 +3073,7 @@
       <c r="K65" s="20"/>
       <c r="L65"/>
     </row>
-    <row r="66" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
         <v>65</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="K66" s="20"/>
       <c r="L66"/>
     </row>
-    <row r="67" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>261</v>
       </c>
@@ -3119,7 +3119,7 @@
       <c r="K67" s="27"/>
       <c r="L67"/>
     </row>
-    <row r="68" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -3142,7 +3142,7 @@
       <c r="K68" s="20"/>
       <c r="L68"/>
     </row>
-    <row r="69" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
@@ -3159,13 +3159,13 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G69" s="20"/>
       <c r="K69" s="20"/>
       <c r="L69"/>
     </row>
-    <row r="70" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>191</v>
       </c>
@@ -3188,7 +3188,7 @@
       <c r="K70" s="20"/>
       <c r="L70"/>
     </row>
-    <row r="71" spans="1:13" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:12" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="24" t="s">
         <v>253</v>
       </c>
@@ -3211,7 +3211,7 @@
       <c r="K71" s="20"/>
       <c r="L71"/>
     </row>
-    <row r="72" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>72</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G72" s="20"/>
       <c r="H72" s="43"/>
@@ -3237,7 +3237,7 @@
       <c r="K72" s="21"/>
       <c r="L72"/>
     </row>
-    <row r="73" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="42" t="s">
         <v>194</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>10</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D73" s="42" t="b">
         <v>0</v>
@@ -3258,15 +3258,15 @@
       <c r="K73" s="20"/>
       <c r="L73"/>
     </row>
-    <row r="74" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A74" s="48" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B74" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C74" s="48" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D74" s="48" t="b">
         <v>0</v>
@@ -3281,7 +3281,7 @@
       <c r="K74" s="27"/>
       <c r="L74"/>
     </row>
-    <row r="75" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A75" s="7" t="s">
         <v>74</v>
       </c>
@@ -3304,16 +3304,16 @@
       <c r="K75" s="20"/>
       <c r="L75"/>
     </row>
-    <row r="76" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="B76" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="B76" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="38" t="s">
-        <v>298</v>
-      </c>
       <c r="D76" s="45" t="b">
         <v>0</v>
       </c>
@@ -3321,12 +3321,12 @@
         <v>1</v>
       </c>
       <c r="F76" s="45" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G76" s="27"/>
-      <c r="M76" s="27"/>
-    </row>
-    <row r="77" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K76" s="27"/>
+    </row>
+    <row r="77" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>217</v>
       </c>
@@ -3349,7 +3349,7 @@
       <c r="K77" s="20"/>
       <c r="L77"/>
     </row>
-    <row r="78" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
@@ -3372,7 +3372,7 @@
       <c r="K78" s="20"/>
       <c r="L78"/>
     </row>
-    <row r="79" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G79" s="20"/>
       <c r="H79" s="43"/>
@@ -3398,7 +3398,7 @@
       <c r="K79" s="21"/>
       <c r="L79"/>
     </row>
-    <row r="80" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>80</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G81" s="20"/>
       <c r="K81" s="20"/>
@@ -3507,7 +3507,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>275</v>
+        <v>313</v>
       </c>
       <c r="G84" s="20"/>
       <c r="J84" s="17"/>
@@ -3702,13 +3702,13 @@
     </row>
     <row r="93" spans="1:12" s="49" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A93" s="49" t="s">
+        <v>306</v>
+      </c>
+      <c r="B93" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="49" t="s">
         <v>307</v>
-      </c>
-      <c r="B93" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="49" t="s">
-        <v>308</v>
       </c>
       <c r="D93" s="49" t="b">
         <v>0</v>
@@ -3765,7 +3765,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G95" s="20"/>
       <c r="I95" s="34"/>
@@ -3798,13 +3798,13 @@
     </row>
     <row r="97" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B97" t="s">
         <v>10</v>
       </c>
       <c r="C97" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D97" t="b">
         <v>1</v>
@@ -3813,7 +3813,7 @@
         <v>1</v>
       </c>
       <c r="F97" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G97" s="27"/>
       <c r="K97" s="27"/>
@@ -3835,7 +3835,7 @@
         <v>1</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G98" s="20"/>
       <c r="K98" s="20"/>
@@ -3924,7 +3924,7 @@
         <v>0</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G102" s="20"/>
       <c r="H102" s="43"/>
@@ -4117,13 +4117,13 @@
     </row>
     <row r="110" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
+        <v>281</v>
+      </c>
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
         <v>282</v>
-      </c>
-      <c r="B110" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" t="s">
-        <v>283</v>
       </c>
       <c r="D110" t="b">
         <v>0</v>
@@ -4235,20 +4235,20 @@
         <v>0</v>
       </c>
       <c r="F114" s="43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G114" s="20"/>
       <c r="K114" s="20"/>
     </row>
     <row r="115" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B115" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C115" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D115" s="44" t="b">
         <v>1</v>
@@ -4256,8 +4256,8 @@
       <c r="E115" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="F115" s="44" t="s">
-        <v>313</v>
+      <c r="F115" s="50" t="s">
+        <v>312</v>
       </c>
       <c r="G115" s="27"/>
       <c r="K115" s="21"/>

</xml_diff>

<commit_message>
Regressietest configuratie toegevoegd in properties bestanden
Voor alle instellingen is per type model een "regtest" kolom opgenomen
waarin de regressietest parameters zijn geplaatst. Deze waarden moeten
worden doorgenomen voor klanten op basis van hun gebruik van Imvertor,
dwz. de producten die zij voeren. Vooralsnog zijn de regetsts ingericht
conform de "uitgebreid" processing mode.

Minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BIJ12/props/BIJ12.xlsx
+++ b/src/main/resources/input/BIJ12/props/BIJ12.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="317">
   <si>
     <t>Name</t>
   </si>
@@ -849,15 +849,6 @@
     <t>respec</t>
   </si>
   <si>
-    <t>SIM: opleveren</t>
-  </si>
-  <si>
-    <t>SIM: minimum</t>
-  </si>
-  <si>
-    <t>SIM: uitgebreid</t>
-  </si>
-  <si>
     <t>createskos</t>
   </si>
   <si>
@@ -967,6 +958,24 @@
   </si>
   <si>
     <t>CM</t>
+  </si>
+  <si>
+    <t>CM: minimum</t>
+  </si>
+  <si>
+    <t>CM: uitgebreid</t>
+  </si>
+  <si>
+    <t>CM: opleveren</t>
+  </si>
+  <si>
+    <t>CM: regtest</t>
+  </si>
+  <si>
+    <t>regression</t>
+  </si>
+  <si>
+    <t>Should a regression test be performed on the results of this run?</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1120,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1216,6 +1225,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1543,13 +1555,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L139"/>
+  <dimension ref="A1:M140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomRight" activeCell="A88" sqref="A88:F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1563,11 +1575,12 @@
     <col min="7" max="7" width="5.4609375" style="23" customWidth="1"/>
     <col min="8" max="9" width="14.765625" customWidth="1"/>
     <col min="10" max="10" width="14.3046875" customWidth="1"/>
-    <col min="11" max="11" width="5.4609375" style="23" customWidth="1"/>
-    <col min="12" max="12" width="27.3046875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.4609375" customWidth="1"/>
+    <col min="12" max="12" width="5.4609375" style="23" customWidth="1"/>
+    <col min="13" max="13" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1596,27 +1609,33 @@
       <c r="J1" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="L1" s="18"/>
+      <c r="M1" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="19"/>
       <c r="H2" s="3" t="s">
-        <v>275</v>
+        <v>311</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>276</v>
+        <v>312</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
+        <v>313</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="L2" s="19"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -1633,10 +1652,11 @@
         <v>1</v>
       </c>
       <c r="G3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3"/>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K3" s="51"/>
+      <c r="L3" s="20"/>
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1656,10 +1676,11 @@
         <v>4</v>
       </c>
       <c r="G4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K4" s="51"/>
+      <c r="L4" s="20"/>
+      <c r="M4"/>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1679,10 +1700,11 @@
         <v>4</v>
       </c>
       <c r="G5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K5" s="51"/>
+      <c r="L5" s="20"/>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>157</v>
       </c>
@@ -1699,39 +1721,41 @@
         <v>1</v>
       </c>
       <c r="G6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="51" t="s">
+      <c r="L6" s="20"/>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="51" t="b">
+      <c r="D7" s="52" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="20"/>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="G8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K8" s="51"/>
+      <c r="L8" s="20"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>160</v>
       </c>
@@ -1751,10 +1775,10 @@
         <v>16</v>
       </c>
       <c r="G9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L9" s="20"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1774,10 +1798,11 @@
         <v>4</v>
       </c>
       <c r="G10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K10" s="51"/>
+      <c r="L10" s="20"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>162</v>
       </c>
@@ -1794,10 +1819,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L11" s="20"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>135</v>
       </c>
@@ -1817,10 +1842,11 @@
         <v>4</v>
       </c>
       <c r="G12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K12" s="51"/>
+      <c r="L12" s="20"/>
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13" t="s">
         <v>243</v>
       </c>
@@ -1840,10 +1866,11 @@
         <v>246</v>
       </c>
       <c r="G13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K13" s="51"/>
+      <c r="L13" s="20"/>
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1863,10 +1890,11 @@
         <v>16</v>
       </c>
       <c r="G14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K14" s="51"/>
+      <c r="L14" s="20"/>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1892,10 +1920,13 @@
       <c r="J15" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K15" s="20"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K15" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="20"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1915,10 +1946,11 @@
         <v>10</v>
       </c>
       <c r="G16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K16" s="51"/>
+      <c r="L16" s="20"/>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>221</v>
       </c>
@@ -1938,10 +1970,11 @@
         <v>222</v>
       </c>
       <c r="G17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K17" s="51"/>
+      <c r="L17" s="20"/>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>223</v>
       </c>
@@ -1954,13 +1987,14 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K18" s="51"/>
+      <c r="L18" s="20"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
@@ -1977,10 +2011,11 @@
         <v>1</v>
       </c>
       <c r="G19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19"/>
-    </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K19" s="51"/>
+      <c r="L19" s="20"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>137</v>
       </c>
@@ -1997,13 +2032,14 @@
         <v>1</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K20" s="51"/>
+      <c r="L20" s="20"/>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>140</v>
       </c>
@@ -2020,13 +2056,14 @@
         <v>1</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21"/>
-    </row>
-    <row r="22" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K21" s="51"/>
+      <c r="L21" s="20"/>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>143</v>
       </c>
@@ -2052,10 +2089,13 @@
       <c r="J22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K22" s="20"/>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K22" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="20"/>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2075,10 +2115,10 @@
         <v>16</v>
       </c>
       <c r="G23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L23" s="20"/>
+      <c r="M23"/>
+    </row>
+    <row r="24" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>166</v>
       </c>
@@ -2095,10 +2135,11 @@
         <v>1</v>
       </c>
       <c r="G24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24"/>
-    </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="K24" s="51"/>
+      <c r="L24" s="20"/>
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -2124,10 +2165,13 @@
       <c r="J25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="20"/>
-      <c r="L25"/>
-    </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K25" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="20"/>
+      <c r="M25"/>
+    </row>
+    <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2153,18 +2197,21 @@
       <c r="J26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K26" s="20"/>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K26" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="20"/>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="46" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D27" s="46" t="b">
         <v>0</v>
@@ -2182,10 +2229,13 @@
       <c r="J27" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K27" s="27"/>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K27" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="27"/>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -2211,10 +2261,13 @@
       <c r="J28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K28" s="20"/>
-      <c r="L28"/>
-    </row>
-    <row r="29" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K28" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="20"/>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>145</v>
       </c>
@@ -2240,10 +2293,13 @@
       <c r="J29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K29" s="20"/>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K29" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="20"/>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="28" t="s">
         <v>259</v>
       </c>
@@ -2265,10 +2321,11 @@
       <c r="G30" s="27"/>
       <c r="I30" s="29"/>
       <c r="J30" s="29"/>
-      <c r="K30" s="27"/>
-      <c r="L30"/>
-    </row>
-    <row r="31" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K30" s="51"/>
+      <c r="L30" s="27"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="30" t="s">
         <v>264</v>
       </c>
@@ -2285,16 +2342,17 @@
         <v>1</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G31" s="27"/>
       <c r="H31" s="31"/>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
-      <c r="K31" s="27"/>
-      <c r="L31"/>
-    </row>
-    <row r="32" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K31" s="51"/>
+      <c r="L31" s="27"/>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
@@ -2320,10 +2378,13 @@
       <c r="J32" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="20"/>
-      <c r="L32"/>
-    </row>
-    <row r="33" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K32" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" s="20"/>
+      <c r="M32"/>
+    </row>
+    <row r="33" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>168</v>
       </c>
@@ -2343,10 +2404,11 @@
         <v>10</v>
       </c>
       <c r="G33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33"/>
-    </row>
-    <row r="34" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K33" s="51"/>
+      <c r="L33" s="20"/>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>171</v>
       </c>
@@ -2366,10 +2428,11 @@
         <v>268</v>
       </c>
       <c r="G34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34"/>
-    </row>
-    <row r="35" spans="1:12" s="36" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K34" s="51"/>
+      <c r="L34" s="20"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="1:13" s="36" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="36" t="s">
         <v>270</v>
       </c>
@@ -2389,9 +2452,10 @@
         <v>273</v>
       </c>
       <c r="G35" s="27"/>
-      <c r="K35" s="27"/>
-    </row>
-    <row r="36" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K35" s="51"/>
+      <c r="L35" s="27"/>
+    </row>
+    <row r="36" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
@@ -2411,18 +2475,19 @@
         <v>16</v>
       </c>
       <c r="G36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36"/>
-    </row>
-    <row r="37" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K36" s="51"/>
+      <c r="L36" s="20"/>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="38" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B37" s="38" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D37" s="38" t="b">
         <v>0</v>
@@ -2434,17 +2499,17 @@
         <v>16</v>
       </c>
       <c r="G37" s="39"/>
-      <c r="K37" s="39"/>
-    </row>
-    <row r="38" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L37" s="39"/>
+    </row>
+    <row r="38" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="48" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B38" s="48" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D38" s="48" t="b">
         <v>0</v>
@@ -2456,9 +2521,10 @@
         <v>16</v>
       </c>
       <c r="G38" s="27"/>
-      <c r="K38" s="27"/>
-    </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="K38" s="51"/>
+      <c r="L38" s="27"/>
+    </row>
+    <row r="39" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -2478,10 +2544,11 @@
         <v>16</v>
       </c>
       <c r="G39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39"/>
-    </row>
-    <row r="40" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K39" s="51"/>
+      <c r="L39" s="20"/>
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
@@ -2501,10 +2568,11 @@
         <v>16</v>
       </c>
       <c r="G40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40"/>
-    </row>
-    <row r="41" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K40" s="51"/>
+      <c r="L40" s="20"/>
+      <c r="M40"/>
+    </row>
+    <row r="41" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -2524,10 +2592,11 @@
         <v>16</v>
       </c>
       <c r="G41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41"/>
-    </row>
-    <row r="42" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K41" s="51"/>
+      <c r="L41" s="20"/>
+      <c r="M41"/>
+    </row>
+    <row r="42" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="30" t="s">
         <v>263</v>
       </c>
@@ -2544,16 +2613,17 @@
         <v>1</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G42" s="27"/>
       <c r="H42" s="35"/>
       <c r="I42" s="37"/>
       <c r="J42" s="37"/>
-      <c r="K42" s="27"/>
-      <c r="L42"/>
-    </row>
-    <row r="43" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K42" s="51"/>
+      <c r="L42" s="27"/>
+      <c r="M42"/>
+    </row>
+    <row r="43" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>174</v>
       </c>
@@ -2579,10 +2649,13 @@
       <c r="J43" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K43" s="20"/>
-      <c r="L43"/>
-    </row>
-    <row r="44" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K43" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="L43" s="20"/>
+      <c r="M43"/>
+    </row>
+    <row r="44" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
@@ -2602,10 +2675,10 @@
         <v>16</v>
       </c>
       <c r="G44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44"/>
-    </row>
-    <row r="45" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L44" s="20"/>
+      <c r="M44"/>
+    </row>
+    <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
         <v>47</v>
       </c>
@@ -2625,20 +2698,20 @@
         <v>218</v>
       </c>
       <c r="G45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45"/>
-    </row>
-    <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="51" t="s">
+      <c r="L45" s="20"/>
+      <c r="M45"/>
+    </row>
+    <row r="46" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="51" t="s">
+      <c r="B46" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="51" t="b">
+      <c r="D46" s="52" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
@@ -2648,19 +2721,21 @@
         <v>16</v>
       </c>
       <c r="G46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46"/>
-    </row>
-    <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="51"/>
-      <c r="B47" s="51"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="20"/>
+      <c r="M46"/>
+    </row>
+    <row r="47" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="52"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
       <c r="G47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47"/>
-    </row>
-    <row r="48" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K47" s="51"/>
+      <c r="L47" s="20"/>
+      <c r="M47"/>
+    </row>
+    <row r="48" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>176</v>
       </c>
@@ -2677,10 +2752,11 @@
         <v>0</v>
       </c>
       <c r="G48" s="20"/>
-      <c r="K48" s="20"/>
-      <c r="L48"/>
-    </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K48" s="51"/>
+      <c r="L48" s="20"/>
+      <c r="M48"/>
+    </row>
+    <row r="49" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
@@ -2697,10 +2773,11 @@
         <v>1</v>
       </c>
       <c r="G49" s="20"/>
-      <c r="K49" s="20"/>
-      <c r="L49"/>
-    </row>
-    <row r="50" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K49" s="51"/>
+      <c r="L49" s="20"/>
+      <c r="M49"/>
+    </row>
+    <row r="50" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -2720,10 +2797,11 @@
         <v>206</v>
       </c>
       <c r="G50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50"/>
-    </row>
-    <row r="51" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K50" s="51"/>
+      <c r="L50" s="21"/>
+      <c r="M50"/>
+    </row>
+    <row r="51" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>219</v>
       </c>
@@ -2736,16 +2814,17 @@
         <v>0</v>
       </c>
       <c r="F51" s="50" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G51" s="21"/>
       <c r="H51" s="43"/>
       <c r="I51" s="43"/>
       <c r="J51" s="43"/>
-      <c r="K51" s="21"/>
-      <c r="L51"/>
-    </row>
-    <row r="52" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K51" s="51"/>
+      <c r="L51" s="21"/>
+      <c r="M51"/>
+    </row>
+    <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
         <v>179</v>
       </c>
@@ -2765,10 +2844,10 @@
         <v>4</v>
       </c>
       <c r="G52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52"/>
-    </row>
-    <row r="53" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L52" s="20"/>
+      <c r="M52"/>
+    </row>
+    <row r="53" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
         <v>181</v>
       </c>
@@ -2788,10 +2867,10 @@
         <v>209</v>
       </c>
       <c r="G53" s="20"/>
-      <c r="K53" s="20"/>
-      <c r="L53"/>
-    </row>
-    <row r="54" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L53" s="20"/>
+      <c r="M53"/>
+    </row>
+    <row r="54" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
@@ -2811,10 +2890,11 @@
         <v>16</v>
       </c>
       <c r="G54" s="20"/>
-      <c r="K54" s="20"/>
-      <c r="L54"/>
-    </row>
-    <row r="55" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K54" s="51"/>
+      <c r="L54" s="20"/>
+      <c r="M54"/>
+    </row>
+    <row r="55" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
@@ -2834,10 +2914,11 @@
         <v>16</v>
       </c>
       <c r="G55" s="20"/>
-      <c r="K55" s="20"/>
-      <c r="L55"/>
-    </row>
-    <row r="56" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K55" s="51"/>
+      <c r="L55" s="20"/>
+      <c r="M55"/>
+    </row>
+    <row r="56" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="7" t="s">
         <v>61</v>
       </c>
@@ -2857,10 +2938,10 @@
         <v>16</v>
       </c>
       <c r="G56" s="20"/>
-      <c r="K56" s="20"/>
-      <c r="L56"/>
-    </row>
-    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L56" s="20"/>
+      <c r="M56"/>
+    </row>
+    <row r="57" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>184</v>
       </c>
@@ -2880,18 +2961,19 @@
         <v>16</v>
       </c>
       <c r="G57" s="20"/>
-      <c r="K57" s="20"/>
-      <c r="L57"/>
-    </row>
-    <row r="58" spans="1:12" s="47" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K57" s="51"/>
+      <c r="L57" s="20"/>
+      <c r="M57"/>
+    </row>
+    <row r="58" spans="1:13" s="47" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="47" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B58" s="47" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="47" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D58" s="47" t="b">
         <v>0</v>
@@ -2909,18 +2991,21 @@
       <c r="J58" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="K58" s="27"/>
-      <c r="L58"/>
-    </row>
-    <row r="59" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="K58" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L58" s="27"/>
+      <c r="M58"/>
+    </row>
+    <row r="59" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B59" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D59" s="16" t="b">
         <v>0</v>
@@ -2933,40 +3018,41 @@
       <c r="H59" s="16"/>
       <c r="I59" s="16"/>
       <c r="J59" s="16"/>
-      <c r="K59" s="22"/>
-      <c r="L59"/>
-    </row>
-    <row r="60" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K59" s="16"/>
+      <c r="L59" s="22"/>
+      <c r="M59"/>
+    </row>
+    <row r="60" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="G60" s="27"/>
+      <c r="L60" s="27"/>
+    </row>
+    <row r="61" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
         <v>286</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="G60" s="27"/>
-      <c r="K60" s="27"/>
-    </row>
-    <row r="61" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
-        <v>289</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D61" s="7" t="b">
         <v>0</v>
@@ -2979,9 +3065,10 @@
       <c r="H61" s="33"/>
       <c r="I61" s="33"/>
       <c r="J61" s="33"/>
-      <c r="K61" s="27"/>
-    </row>
-    <row r="62" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K61" s="33"/>
+      <c r="L61" s="27"/>
+    </row>
+    <row r="62" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
         <v>186</v>
       </c>
@@ -2998,10 +3085,10 @@
         <v>1</v>
       </c>
       <c r="G62" s="20"/>
-      <c r="K62" s="20"/>
-      <c r="L62"/>
-    </row>
-    <row r="63" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L62" s="20"/>
+      <c r="M62"/>
+    </row>
+    <row r="63" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A63" s="16" t="s">
         <v>239</v>
       </c>
@@ -3024,10 +3111,11 @@
       <c r="H63" s="16"/>
       <c r="I63" s="16"/>
       <c r="J63" s="16"/>
-      <c r="K63" s="22"/>
-      <c r="L63"/>
-    </row>
-    <row r="64" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K63" s="16"/>
+      <c r="L63" s="22"/>
+      <c r="M63"/>
+    </row>
+    <row r="64" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A64" s="7" t="s">
         <v>188</v>
       </c>
@@ -3047,10 +3135,10 @@
         <v>19</v>
       </c>
       <c r="G64" s="20"/>
-      <c r="K64" s="20"/>
-      <c r="L64"/>
-    </row>
-    <row r="65" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L64" s="20"/>
+      <c r="M64"/>
+    </row>
+    <row r="65" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -3070,10 +3158,11 @@
         <v>207</v>
       </c>
       <c r="G65" s="20"/>
-      <c r="K65" s="20"/>
-      <c r="L65"/>
-    </row>
-    <row r="66" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K65" s="51"/>
+      <c r="L65" s="20"/>
+      <c r="M65"/>
+    </row>
+    <row r="66" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
         <v>65</v>
       </c>
@@ -3093,10 +3182,10 @@
         <v>218</v>
       </c>
       <c r="G66" s="20"/>
-      <c r="K66" s="20"/>
-      <c r="L66"/>
-    </row>
-    <row r="67" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L66" s="20"/>
+      <c r="M66"/>
+    </row>
+    <row r="67" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>261</v>
       </c>
@@ -3116,10 +3205,10 @@
         <v>226</v>
       </c>
       <c r="G67" s="27"/>
-      <c r="K67" s="27"/>
-      <c r="L67"/>
-    </row>
-    <row r="68" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L67" s="27"/>
+      <c r="M67"/>
+    </row>
+    <row r="68" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -3139,10 +3228,11 @@
         <v>210</v>
       </c>
       <c r="G68" s="20"/>
-      <c r="K68" s="20"/>
-      <c r="L68"/>
-    </row>
-    <row r="69" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K68" s="51"/>
+      <c r="L68" s="20"/>
+      <c r="M68"/>
+    </row>
+    <row r="69" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
@@ -3159,13 +3249,14 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G69" s="20"/>
-      <c r="K69" s="20"/>
-      <c r="L69"/>
-    </row>
-    <row r="70" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K69" s="51"/>
+      <c r="L69" s="20"/>
+      <c r="M69"/>
+    </row>
+    <row r="70" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>191</v>
       </c>
@@ -3185,10 +3276,11 @@
         <v>208</v>
       </c>
       <c r="G70" s="20"/>
-      <c r="K70" s="20"/>
-      <c r="L70"/>
-    </row>
-    <row r="71" spans="1:12" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K70" s="51"/>
+      <c r="L70" s="20"/>
+      <c r="M70"/>
+    </row>
+    <row r="71" spans="1:13" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="24" t="s">
         <v>253</v>
       </c>
@@ -3208,10 +3300,11 @@
         <v>254</v>
       </c>
       <c r="G71" s="20"/>
-      <c r="K71" s="20"/>
-      <c r="L71"/>
-    </row>
-    <row r="72" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K71" s="51"/>
+      <c r="L71" s="20"/>
+      <c r="M71"/>
+    </row>
+    <row r="72" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>72</v>
       </c>
@@ -3228,16 +3321,17 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G72" s="20"/>
       <c r="H72" s="43"/>
       <c r="I72" s="43"/>
       <c r="J72" s="43"/>
-      <c r="K72" s="21"/>
-      <c r="L72"/>
-    </row>
-    <row r="73" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K72" s="51"/>
+      <c r="L72" s="21"/>
+      <c r="M72"/>
+    </row>
+    <row r="73" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="42" t="s">
         <v>194</v>
       </c>
@@ -3245,7 +3339,7 @@
         <v>10</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D73" s="42" t="b">
         <v>0</v>
@@ -3255,18 +3349,19 @@
       </c>
       <c r="F73" s="42"/>
       <c r="G73" s="20"/>
-      <c r="K73" s="20"/>
-      <c r="L73"/>
-    </row>
-    <row r="74" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K73" s="51"/>
+      <c r="L73" s="20"/>
+      <c r="M73"/>
+    </row>
+    <row r="74" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A74" s="48" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B74" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C74" s="48" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D74" s="48" t="b">
         <v>0</v>
@@ -3278,10 +3373,11 @@
         <v>226</v>
       </c>
       <c r="G74" s="27"/>
-      <c r="K74" s="27"/>
-      <c r="L74"/>
-    </row>
-    <row r="75" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K74" s="51"/>
+      <c r="L74" s="27"/>
+      <c r="M74"/>
+    </row>
+    <row r="75" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A75" s="7" t="s">
         <v>74</v>
       </c>
@@ -3301,18 +3397,18 @@
         <v>4</v>
       </c>
       <c r="G75" s="20"/>
-      <c r="K75" s="20"/>
-      <c r="L75"/>
-    </row>
-    <row r="76" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L75" s="20"/>
+      <c r="M75"/>
+    </row>
+    <row r="76" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="38" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B76" s="38" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="38" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D76" s="45" t="b">
         <v>0</v>
@@ -3324,9 +3420,9 @@
         <v>16</v>
       </c>
       <c r="G76" s="27"/>
-      <c r="K76" s="27"/>
-    </row>
-    <row r="77" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L76" s="27"/>
+    </row>
+    <row r="77" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>217</v>
       </c>
@@ -3346,10 +3442,11 @@
         <v>16</v>
       </c>
       <c r="G77" s="20"/>
-      <c r="K77" s="20"/>
-      <c r="L77"/>
-    </row>
-    <row r="78" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K77" s="51"/>
+      <c r="L77" s="20"/>
+      <c r="M77"/>
+    </row>
+    <row r="78" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
@@ -3369,10 +3466,11 @@
         <v>4</v>
       </c>
       <c r="G78" s="20"/>
-      <c r="K78" s="20"/>
-      <c r="L78"/>
-    </row>
-    <row r="79" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K78" s="51"/>
+      <c r="L78" s="20"/>
+      <c r="M78"/>
+    </row>
+    <row r="79" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -3389,16 +3487,17 @@
         <v>0</v>
       </c>
       <c r="F79" s="50" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G79" s="20"/>
       <c r="H79" s="43"/>
       <c r="I79" s="43"/>
       <c r="J79" s="43"/>
-      <c r="K79" s="21"/>
-      <c r="L79"/>
-    </row>
-    <row r="80" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K79" s="51"/>
+      <c r="L79" s="21"/>
+      <c r="M79"/>
+    </row>
+    <row r="80" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>80</v>
       </c>
@@ -3418,10 +3517,11 @@
         <v>269</v>
       </c>
       <c r="G80" s="20"/>
-      <c r="K80" s="20"/>
-      <c r="L80"/>
-    </row>
-    <row r="81" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K80" s="51"/>
+      <c r="L80" s="20"/>
+      <c r="M80"/>
+    </row>
+    <row r="81" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="7" t="s">
         <v>83</v>
       </c>
@@ -3438,13 +3538,13 @@
         <v>0</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G81" s="20"/>
-      <c r="K81" s="20"/>
-      <c r="L81"/>
-    </row>
-    <row r="82" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L81" s="20"/>
+      <c r="M81"/>
+    </row>
+    <row r="82" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>195</v>
       </c>
@@ -3464,10 +3564,11 @@
         <v>19</v>
       </c>
       <c r="G82" s="20"/>
-      <c r="K82" s="20"/>
-      <c r="L82"/>
-    </row>
-    <row r="83" spans="1:12" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="K82" s="51"/>
+      <c r="L82" s="20"/>
+      <c r="M82"/>
+    </row>
+    <row r="83" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
         <v>198</v>
       </c>
@@ -3487,10 +3588,10 @@
         <v>211</v>
       </c>
       <c r="G83" s="20"/>
-      <c r="K83" s="20"/>
-      <c r="L83"/>
-    </row>
-    <row r="84" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L83" s="20"/>
+      <c r="M83"/>
+    </row>
+    <row r="84" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>85</v>
       </c>
@@ -3507,14 +3608,15 @@
         <v>0</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G84" s="20"/>
       <c r="J84" s="17"/>
-      <c r="K84" s="20"/>
-      <c r="L84"/>
-    </row>
-    <row r="85" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K84" s="51"/>
+      <c r="L84" s="20"/>
+      <c r="M84"/>
+    </row>
+    <row r="85" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>87</v>
       </c>
@@ -3534,10 +3636,11 @@
         <v>88</v>
       </c>
       <c r="G85" s="20"/>
-      <c r="K85" s="20"/>
-      <c r="L85"/>
-    </row>
-    <row r="86" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="K85" s="51"/>
+      <c r="L85" s="20"/>
+      <c r="M85"/>
+    </row>
+    <row r="86" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="7" t="s">
         <v>91</v>
       </c>
@@ -3557,10 +3660,10 @@
         <v>92</v>
       </c>
       <c r="G86" s="20"/>
-      <c r="K86" s="20"/>
-      <c r="L86"/>
-    </row>
-    <row r="87" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="L86" s="20"/>
+      <c r="M86"/>
+    </row>
+    <row r="87" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A87" s="7" t="s">
         <v>148</v>
       </c>
@@ -3580,391 +3683,415 @@
         <v>16</v>
       </c>
       <c r="G87" s="20"/>
-      <c r="K87" s="20"/>
-      <c r="L87"/>
-    </row>
-    <row r="88" spans="1:12" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
+      <c r="L87" s="20"/>
+      <c r="M87"/>
+    </row>
+    <row r="88" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="B88" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="D88" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G88" s="39"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="38"/>
+      <c r="J88" s="38"/>
+      <c r="K88" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="L88" s="27"/>
+      <c r="M88"/>
+    </row>
+    <row r="89" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" s="2" t="s">
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G88" s="20"/>
-      <c r="K88" s="20"/>
-      <c r="L88"/>
-    </row>
-    <row r="89" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
+      <c r="G89" s="20"/>
+      <c r="K89" s="51"/>
+      <c r="L89" s="20"/>
+      <c r="M89"/>
+    </row>
+    <row r="90" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B89" s="8"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G89" s="20"/>
-      <c r="H89" s="2" t="s">
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G90" s="20"/>
+      <c r="H90" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I89" s="2" t="s">
+      <c r="I90" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J89" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K89" s="20"/>
-      <c r="L89"/>
-    </row>
-    <row r="90" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
+      <c r="J90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K90" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L90" s="20"/>
+      <c r="M90"/>
+    </row>
+    <row r="91" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="2" t="s">
+      <c r="B91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G90" s="20"/>
-      <c r="K90" s="20"/>
-      <c r="L90"/>
-    </row>
-    <row r="91" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="31" t="s">
+      <c r="D91" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G91" s="20"/>
+      <c r="K91" s="51"/>
+      <c r="L91" s="20"/>
+      <c r="M91"/>
+    </row>
+    <row r="92" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="B91" s="31" t="s">
+      <c r="B92" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="31" t="s">
+      <c r="C92" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="D91" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F91" s="31" t="s">
+      <c r="D92" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="G91" s="27"/>
-      <c r="K91" s="27"/>
-      <c r="L91"/>
-    </row>
-    <row r="92" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
+      <c r="G92" s="27"/>
+      <c r="K92" s="51"/>
+      <c r="L92" s="27"/>
+      <c r="M92"/>
+    </row>
+    <row r="93" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D92" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="12" t="s">
+      <c r="D93" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="G92" s="20"/>
-      <c r="K92" s="20"/>
-      <c r="L92"/>
-    </row>
-    <row r="93" spans="1:12" s="49" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="49" t="s">
-        <v>306</v>
-      </c>
-      <c r="B93" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="49" t="s">
-        <v>307</v>
-      </c>
-      <c r="D93" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="49" t="s">
+      <c r="G93" s="20"/>
+      <c r="K93" s="51"/>
+      <c r="L93" s="20"/>
+      <c r="M93"/>
+    </row>
+    <row r="94" spans="1:13" s="49" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A94" s="49" t="s">
+        <v>303</v>
+      </c>
+      <c r="B94" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="49" t="s">
+        <v>304</v>
+      </c>
+      <c r="D94" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="G93" s="27"/>
-      <c r="I93" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="J93" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="K93" s="27"/>
-      <c r="L93"/>
-    </row>
-    <row r="94" spans="1:12" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="14" t="s">
+      <c r="G94" s="27"/>
+      <c r="I94" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="J94" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="K94" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L94" s="27"/>
+      <c r="M94"/>
+    </row>
+    <row r="95" spans="1:13" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B95" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="C94" s="14" t="s">
+      <c r="C95" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="D94" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="6" t="s">
+      <c r="D95" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="G94" s="20"/>
-      <c r="K94" s="20"/>
-      <c r="L94"/>
-    </row>
-    <row r="95" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
+      <c r="G95" s="20"/>
+      <c r="K95" s="51"/>
+      <c r="L95" s="20"/>
+      <c r="M95"/>
+    </row>
+    <row r="96" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="17" t="s">
-        <v>308</v>
-      </c>
-      <c r="G95" s="20"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="34"/>
-      <c r="K95" s="20"/>
-      <c r="L95"/>
-    </row>
-    <row r="96" spans="1:12" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="2" t="s">
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="G96" s="20"/>
+      <c r="I96" s="34"/>
+      <c r="J96" s="34"/>
+      <c r="K96" s="51"/>
+      <c r="L96" s="20"/>
+      <c r="M96"/>
+    </row>
+    <row r="97" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="2" t="s">
+      <c r="B97" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="2" t="s">
+      <c r="D97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G96" s="20"/>
-      <c r="K96" s="20"/>
-      <c r="L96"/>
-    </row>
-    <row r="97" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A97" t="s">
-        <v>279</v>
-      </c>
-      <c r="B97" t="s">
+      <c r="G97" s="20"/>
+      <c r="K97" s="51"/>
+      <c r="L97" s="20"/>
+      <c r="M97"/>
+    </row>
+    <row r="98" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A98" t="s">
+        <v>276</v>
+      </c>
+      <c r="B98" t="s">
         <v>10</v>
       </c>
-      <c r="C97" t="s">
-        <v>280</v>
-      </c>
-      <c r="D97" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" t="s">
-        <v>308</v>
-      </c>
-      <c r="G97" s="27"/>
-      <c r="K97" s="27"/>
-    </row>
-    <row r="98" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
+      <c r="C98" t="s">
+        <v>277</v>
+      </c>
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" t="s">
+        <v>305</v>
+      </c>
+      <c r="G98" s="27"/>
+      <c r="L98" s="27"/>
+    </row>
+    <row r="99" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D98" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="G98" s="20"/>
-      <c r="K98" s="20"/>
-      <c r="L98"/>
-    </row>
-    <row r="99" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A99" s="2" t="s">
+      <c r="D99" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="G99" s="20"/>
+      <c r="K99" s="51"/>
+      <c r="L99" s="20"/>
+      <c r="M99"/>
+    </row>
+    <row r="100" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="2" t="s">
+      <c r="B100" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D99" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="2" t="s">
+      <c r="D100" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G99" s="20"/>
-      <c r="K99" s="20"/>
-      <c r="L99"/>
-    </row>
-    <row r="100" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
+      <c r="G100" s="20"/>
+      <c r="K100" s="51"/>
+      <c r="L100" s="20"/>
+      <c r="M100"/>
+    </row>
+    <row r="101" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="2" t="s">
+      <c r="B101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G100" s="20"/>
-      <c r="K100" s="20"/>
-      <c r="L100"/>
-    </row>
-    <row r="101" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
+      <c r="D101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G101" s="20"/>
+      <c r="K101" s="51"/>
+      <c r="L101" s="20"/>
+      <c r="M101"/>
+    </row>
+    <row r="102" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" s="2" t="s">
+      <c r="D102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G101" s="20"/>
-      <c r="K101" s="20"/>
-      <c r="L101"/>
-    </row>
-    <row r="102" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
+      <c r="G102" s="20"/>
+      <c r="K102" s="51"/>
+      <c r="L102" s="20"/>
+      <c r="M102"/>
+    </row>
+    <row r="103" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="G102" s="20"/>
-      <c r="H102" s="43"/>
-      <c r="I102" s="43"/>
-      <c r="J102" s="43"/>
-      <c r="K102" s="21"/>
-      <c r="L102"/>
-    </row>
-    <row r="103" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="7" t="s">
+      <c r="D103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="G103" s="20"/>
+      <c r="H103" s="43"/>
+      <c r="I103" s="43"/>
+      <c r="J103" s="43"/>
+      <c r="K103" s="51"/>
+      <c r="L103" s="21"/>
+      <c r="M103"/>
+    </row>
+    <row r="104" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B104" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C104" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D103" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G103" s="20"/>
-      <c r="K103" s="20"/>
-      <c r="L103"/>
-    </row>
-    <row r="104" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="D104" s="7" t="b">
         <v>1</v>
@@ -3976,73 +4103,67 @@
         <v>218</v>
       </c>
       <c r="G104" s="20"/>
-      <c r="K104" s="20"/>
-      <c r="L104"/>
-    </row>
-    <row r="105" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L104" s="20"/>
+      <c r="M104"/>
+    </row>
+    <row r="105" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D105" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="G105" s="20"/>
+      <c r="L105" s="20"/>
+      <c r="M105"/>
+    </row>
+    <row r="106" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B105" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="7" t="s">
+      <c r="B106" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D105" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" s="7" t="s">
+      <c r="D106" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G105" s="20"/>
-      <c r="K105" s="20"/>
-      <c r="L105"/>
-    </row>
-    <row r="106" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="2" t="s">
+      <c r="G106" s="20"/>
+      <c r="L106" s="20"/>
+      <c r="M106"/>
+    </row>
+    <row r="107" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" s="2" t="s">
+      <c r="B107" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D106" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E106" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G106" s="20"/>
-      <c r="H106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K106" s="20"/>
-      <c r="L106"/>
-    </row>
-    <row r="107" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="D107" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107" s="2" t="b">
         <v>1</v>
@@ -4057,148 +4178,160 @@
       <c r="J107" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K107" s="20"/>
-      <c r="L107"/>
-    </row>
-    <row r="108" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K107" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L107" s="20"/>
+      <c r="M107"/>
+    </row>
+    <row r="108" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D108" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G108" s="20"/>
       <c r="H108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L108" s="20"/>
+      <c r="M108"/>
+    </row>
+    <row r="109" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D109" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" s="20"/>
+      <c r="H109" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K108" s="20"/>
-      <c r="L108"/>
-    </row>
-    <row r="109" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A109" s="2" t="s">
+      <c r="I109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L109" s="20"/>
+      <c r="M109"/>
+    </row>
+    <row r="110" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="2" t="s">
+      <c r="B110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D109" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G109" s="20"/>
-      <c r="H109"/>
-      <c r="I109"/>
-      <c r="J109"/>
-      <c r="K109" s="20"/>
-      <c r="L109"/>
-    </row>
-    <row r="110" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" t="s">
-        <v>281</v>
-      </c>
-      <c r="B110" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" t="s">
-        <v>282</v>
-      </c>
-      <c r="D110" t="b">
-        <v>0</v>
-      </c>
-      <c r="E110" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" t="s">
-        <v>4</v>
-      </c>
-      <c r="G110" s="27"/>
+      <c r="D110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G110" s="20"/>
       <c r="H110"/>
       <c r="I110"/>
       <c r="J110"/>
-      <c r="K110" s="27"/>
-    </row>
-    <row r="111" spans="1:12" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A111" s="7" t="s">
+      <c r="K110"/>
+      <c r="L110" s="20"/>
+      <c r="M110"/>
+    </row>
+    <row r="111" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
+        <v>278</v>
+      </c>
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>279</v>
+      </c>
+      <c r="D111" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" t="s">
+        <v>4</v>
+      </c>
+      <c r="G111" s="27"/>
+      <c r="H111"/>
+      <c r="I111"/>
+      <c r="J111"/>
+      <c r="K111"/>
+      <c r="L111" s="27"/>
+    </row>
+    <row r="112" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A112" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B112" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C112" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D111" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111" s="7" t="s">
+      <c r="D112" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G111" s="20"/>
-      <c r="K111" s="20"/>
-    </row>
-    <row r="112" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="2" t="s">
+      <c r="G112" s="20"/>
+      <c r="L112" s="20"/>
+    </row>
+    <row r="113" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="2" t="s">
+      <c r="B113" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="D112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G112" s="20"/>
-      <c r="H112" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K112" s="20"/>
-    </row>
-    <row r="113" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D113" s="2" t="b">
         <v>1</v>
@@ -4216,164 +4349,202 @@
       <c r="J113" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K113" s="20"/>
-    </row>
-    <row r="114" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="K113" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L113" s="20"/>
+    </row>
+    <row r="114" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G114" s="20"/>
+      <c r="H114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K114" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="L114" s="20"/>
+    </row>
+    <row r="115" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F114" s="43" t="s">
-        <v>308</v>
-      </c>
-      <c r="G114" s="20"/>
-      <c r="K114" s="20"/>
-    </row>
-    <row r="115" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="44" t="s">
-        <v>294</v>
-      </c>
-      <c r="B115" s="44" t="s">
+      <c r="D115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" s="43" t="s">
+        <v>305</v>
+      </c>
+      <c r="G115" s="20"/>
+      <c r="K115" s="51"/>
+      <c r="L115" s="20"/>
+    </row>
+    <row r="116" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="B116" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C115" s="44" t="s">
-        <v>295</v>
-      </c>
-      <c r="D115" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" s="50" t="s">
-        <v>312</v>
-      </c>
-      <c r="G115" s="27"/>
-      <c r="K115" s="21"/>
-    </row>
-    <row r="116" spans="1:12" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A116" s="26" t="s">
+      <c r="C116" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="D116" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="G116" s="27"/>
+      <c r="K116" s="51"/>
+      <c r="L116" s="21"/>
+    </row>
+    <row r="117" spans="1:13" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A117" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="B116" s="26" t="s">
+      <c r="B117" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C116" s="26" t="s">
+      <c r="C117" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="D116" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" s="26" t="s">
+      <c r="D117" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="G116" s="27"/>
-      <c r="H116" s="26"/>
-      <c r="I116" s="26"/>
-      <c r="J116" s="26"/>
-      <c r="K116" s="27"/>
-    </row>
-    <row r="117" spans="1:12" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A117" s="2" t="s">
+      <c r="G117" s="27"/>
+      <c r="H117" s="26"/>
+      <c r="I117" s="26"/>
+      <c r="J117" s="26"/>
+      <c r="K117" s="51"/>
+      <c r="L117" s="27"/>
+    </row>
+    <row r="118" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A118" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D117" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F117" s="2" t="s">
+      <c r="D118" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G117" s="20"/>
-      <c r="K117" s="20"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L118"/>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L119"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L120"/>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L121"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L122"/>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L123"/>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L124"/>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L125"/>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L126"/>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L127"/>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="L128"/>
-    </row>
-    <row r="129" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L129"/>
-    </row>
-    <row r="130" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L130"/>
-    </row>
-    <row r="131" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L131"/>
-    </row>
-    <row r="132" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L132"/>
-    </row>
-    <row r="133" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L133"/>
-    </row>
-    <row r="134" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L134"/>
-    </row>
-    <row r="135" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L135"/>
-    </row>
-    <row r="136" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L136"/>
-    </row>
-    <row r="137" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L137"/>
-    </row>
-    <row r="138" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L138"/>
-    </row>
-    <row r="139" spans="12:12" x14ac:dyDescent="0.4">
-      <c r="L139"/>
+      <c r="G118" s="20"/>
+      <c r="K118" s="51"/>
+      <c r="L118" s="20"/>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M119"/>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M120"/>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M121"/>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M122"/>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M123"/>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M124"/>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M125"/>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M126"/>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M127"/>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M128"/>
+    </row>
+    <row r="129" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M129"/>
+    </row>
+    <row r="130" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M130"/>
+    </row>
+    <row r="131" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M131"/>
+    </row>
+    <row r="132" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M132"/>
+    </row>
+    <row r="133" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M133"/>
+    </row>
+    <row r="134" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M134"/>
+    </row>
+    <row r="135" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M135"/>
+    </row>
+    <row r="136" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M136"/>
+    </row>
+    <row r="137" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M137"/>
+    </row>
+    <row r="138" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M138"/>
+    </row>
+    <row r="139" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M139"/>
+    </row>
+    <row r="140" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M140"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
BIJ12: Verbetering inrichting properties (XSLX)
Minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BIJ12/props/BIJ12.xlsx
+++ b/src/main/resources/input/BIJ12/props/BIJ12.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="317">
   <si>
     <t>Name</t>
   </si>
@@ -1558,10 +1558,10 @@
   <dimension ref="A1:M140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A88" sqref="A88:F88"/>
+      <selection pane="bottomRight" activeCell="J117" sqref="J117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1910,19 +1910,14 @@
       <c r="E15" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G15" s="20"/>
-      <c r="H15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="J15" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K15" s="51" t="s">
-        <v>19</v>
-      </c>
+      <c r="K15" s="51"/>
       <c r="L15" s="20"/>
       <c r="M15"/>
     </row>
@@ -2079,15 +2074,12 @@
       <c r="E22" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F22" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G22" s="20"/>
       <c r="H22" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="K22" s="51" t="s">
         <v>16</v>
@@ -2155,19 +2147,11 @@
       <c r="E25" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F25" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G25" s="20"/>
-      <c r="H25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" s="51" t="s">
-        <v>16</v>
-      </c>
+      <c r="K25" s="51"/>
       <c r="L25" s="20"/>
       <c r="M25"/>
     </row>
@@ -2187,19 +2171,14 @@
       <c r="E26" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F26" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G26" s="20"/>
       <c r="H26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K26" s="51"/>
       <c r="L26" s="20"/>
       <c r="M26"/>
     </row>
@@ -2219,19 +2198,14 @@
       <c r="E27" s="46" t="b">
         <v>1</v>
       </c>
+      <c r="F27" s="46" t="s">
+        <v>4</v>
+      </c>
       <c r="G27" s="27"/>
       <c r="H27" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K27" s="51"/>
       <c r="L27" s="27"/>
       <c r="M27"/>
     </row>
@@ -2251,19 +2225,11 @@
       <c r="E28" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F28" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G28" s="20"/>
-      <c r="H28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K28" s="51"/>
       <c r="L28" s="20"/>
       <c r="M28"/>
     </row>
@@ -2283,19 +2249,14 @@
       <c r="E29" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F29" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G29" s="20"/>
       <c r="H29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K29" s="51"/>
       <c r="L29" s="20"/>
       <c r="M29"/>
     </row>
@@ -2368,19 +2329,13 @@
       <c r="E32" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F32" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G32" s="20"/>
-      <c r="H32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="J32" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32" s="51" t="s">
-        <v>34</v>
-      </c>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="51"/>
       <c r="L32" s="20"/>
       <c r="M32"/>
     </row>
@@ -2639,19 +2594,13 @@
       <c r="E43" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F43" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G43" s="20"/>
-      <c r="H43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="J43" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="51" t="s">
-        <v>16</v>
-      </c>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="51"/>
       <c r="L43" s="20"/>
       <c r="M43"/>
     </row>
@@ -2982,18 +2931,13 @@
         <v>1</v>
       </c>
       <c r="F58" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="27"/>
+      <c r="H58" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="G58" s="27"/>
-      <c r="I58" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J58" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="K58" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K58" s="51"/>
       <c r="L58" s="27"/>
       <c r="M58"/>
     </row>
@@ -3751,19 +3695,14 @@
       <c r="E90" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F90" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G90" s="20"/>
-      <c r="H90" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="J90" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K90" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K90" s="51"/>
       <c r="L90" s="20"/>
       <c r="M90"/>
     </row>
@@ -3856,18 +3795,13 @@
         <v>1</v>
       </c>
       <c r="F94" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="G94" s="27"/>
+      <c r="H94" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="G94" s="27"/>
-      <c r="I94" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="J94" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="K94" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K94" s="51"/>
       <c r="L94" s="27"/>
       <c r="M94"/>
     </row>
@@ -4168,19 +4102,11 @@
       <c r="E107" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F107" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G107" s="20"/>
-      <c r="H107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K107" s="51"/>
       <c r="L107" s="20"/>
       <c r="M107"/>
     </row>
@@ -4200,19 +4126,11 @@
       <c r="E108" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F108" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G108" s="20"/>
-      <c r="H108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K108" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K108" s="51"/>
       <c r="L108" s="20"/>
       <c r="M108"/>
     </row>
@@ -4232,19 +4150,14 @@
       <c r="E109" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F109" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G109" s="20"/>
       <c r="H109" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K109" s="51"/>
       <c r="L109" s="20"/>
       <c r="M109"/>
     </row>
@@ -4339,19 +4252,14 @@
       <c r="E113" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F113" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G113" s="20"/>
       <c r="H113" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J113" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K113" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K113" s="51"/>
       <c r="L113" s="20"/>
     </row>
     <row r="114" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -4370,19 +4278,14 @@
       <c r="E114" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F114" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G114" s="20"/>
       <c r="H114" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K114" s="51" t="s">
-        <v>4</v>
-      </c>
+      <c r="K114" s="51"/>
       <c r="L114" s="20"/>
     </row>
     <row r="115" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
MIM 1.2 introductie van "MIM versie" tagged value
Complete rework van configuraties en bestandsnamen.

Zie #503

Minor. Verandering van aanpak, niet van functionaliteit.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BIJ12/props/BIJ12.xlsx
+++ b/src/main/resources/input/BIJ12/props/BIJ12.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\BIJ12\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2236A2CA-6C2F-4067-866E-E698D00F5859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12060"/>
+    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BIJ12" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="327">
   <si>
     <t>Name</t>
   </si>
@@ -954,9 +955,6 @@
     <t>BIJ12_GEOSTANDAARDEN</t>
   </si>
   <si>
-    <t>BIJ12CM</t>
-  </si>
-  <si>
     <t>CM</t>
   </si>
   <si>
@@ -976,12 +974,45 @@
   </si>
   <si>
     <t>Should a regression test be performed on the results of this run?</t>
+  </si>
+  <si>
+    <t>metamodelname</t>
+  </si>
+  <si>
+    <t>Name of the metamodel. When this is a MIM model, specify MIM</t>
+  </si>
+  <si>
+    <t>MIM</t>
+  </si>
+  <si>
+    <t>metamodelversion</t>
+  </si>
+  <si>
+    <t>Version of the metamodel. When this is a MIM model, specify the MIM version</t>
+  </si>
+  <si>
+    <t>metamodelextension</t>
+  </si>
+  <si>
+    <t>Name of the extension. When this is a MIM model, specify the MIM extension name</t>
+  </si>
+  <si>
+    <t>CONCEPTUAL</t>
+  </si>
+  <si>
+    <t>metamodelextensionversion</t>
+  </si>
+  <si>
+    <t>Vetsion of the extension. When this is a MIM model, specify the MIM extension version</t>
+  </si>
+  <si>
+    <t>1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1120,7 +1151,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1148,22 +1179,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
@@ -1179,46 +1198,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
@@ -1230,51 +1210,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
-    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
-    <cellStyle name="Good" xfId="5" builtinId="26"/>
+    <cellStyle name="Controlecel" xfId="2" builtinId="23"/>
+    <cellStyle name="Goed" xfId="5" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Ongeldig" xfId="3" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="4" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1551,17 +1495,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M140"/>
+  <dimension ref="A1:T144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J117" sqref="J117"/>
+      <selection pane="bottomRight" activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1572,11 +1516,11 @@
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="5.4609375" style="23" customWidth="1"/>
+    <col min="7" max="7" width="5.4609375" style="19" customWidth="1"/>
     <col min="8" max="9" width="14.765625" customWidth="1"/>
     <col min="10" max="10" width="14.3046875" customWidth="1"/>
     <col min="11" max="11" width="12.4609375" customWidth="1"/>
-    <col min="12" max="12" width="5.4609375" style="23" customWidth="1"/>
+    <col min="12" max="12" width="5.4609375" style="19" customWidth="1"/>
     <col min="13" max="13" width="27.3046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1599,7 +1543,7 @@
       <c r="F1" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="18"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="4" t="s">
         <v>252</v>
       </c>
@@ -1612,27 +1556,27 @@
       <c r="K1" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="L1" s="18"/>
+      <c r="L1" s="14"/>
       <c r="M1" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
-      <c r="G2" s="19"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="L2" s="19"/>
+      <c r="L2" s="15"/>
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
@@ -1651,9 +1595,8 @@
       <c r="E3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="20"/>
+      <c r="G3" s="16"/>
+      <c r="L3" s="16"/>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1675,9 +1618,8 @@
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="20"/>
+      <c r="G4" s="16"/>
+      <c r="L4" s="16"/>
       <c r="M4"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1699,9 +1641,8 @@
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="20"/>
+      <c r="G5" s="16"/>
+      <c r="L5" s="16"/>
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -1720,39 +1661,37 @@
       <c r="E6" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="G6" s="16"/>
+      <c r="L6" s="16"/>
       <c r="M6"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="52" t="b">
+      <c r="D7" s="23" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="20"/>
+      <c r="G7" s="16"/>
+      <c r="L7" s="16"/>
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="G8" s="20"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="20"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="G8" s="16"/>
+      <c r="L8" s="16"/>
       <c r="M8"/>
     </row>
     <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -1774,8 +1713,8 @@
       <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="G9" s="16"/>
+      <c r="L9" s="16"/>
       <c r="M9"/>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1797,9 +1736,8 @@
       <c r="F10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="20"/>
+      <c r="G10" s="16"/>
+      <c r="L10" s="16"/>
       <c r="M10"/>
     </row>
     <row r="11" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1818,8 +1756,8 @@
       <c r="E11" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="G11" s="16"/>
+      <c r="L11" s="16"/>
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1841,33 +1779,31 @@
       <c r="F12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="20"/>
+      <c r="G12" s="16"/>
+      <c r="L12" s="16"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D13" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="20"/>
+      <c r="G13" s="16"/>
+      <c r="L13" s="16"/>
       <c r="M13"/>
     </row>
     <row r="14" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1889,9 +1825,8 @@
       <c r="F14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="20"/>
+      <c r="G14" s="16"/>
+      <c r="L14" s="16"/>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1913,12 +1848,11 @@
       <c r="F15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="G15" s="16"/>
       <c r="J15" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K15" s="51"/>
-      <c r="L15" s="20"/>
+      <c r="L15" s="16"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1940,9 +1874,8 @@
       <c r="F16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="20"/>
+      <c r="G16" s="16"/>
+      <c r="L16" s="16"/>
       <c r="M16"/>
     </row>
     <row r="17" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1964,9 +1897,8 @@
       <c r="F17" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="20"/>
+      <c r="G17" s="16"/>
+      <c r="L17" s="16"/>
       <c r="M17"/>
     </row>
     <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1984,9 +1916,8 @@
       <c r="F18" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="20"/>
+      <c r="G18" s="16"/>
+      <c r="L18" s="16"/>
       <c r="M18"/>
     </row>
     <row r="19" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2005,9 +1936,8 @@
       <c r="E19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="20"/>
+      <c r="G19" s="16"/>
+      <c r="L19" s="16"/>
       <c r="M19"/>
     </row>
     <row r="20" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2026,12 +1956,11 @@
       <c r="E20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="20"/>
+      <c r="G20" s="16"/>
+      <c r="L20" s="16"/>
       <c r="M20"/>
     </row>
     <row r="21" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2050,12 +1979,11 @@
       <c r="E21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="20"/>
+      <c r="G21" s="16"/>
+      <c r="L21" s="16"/>
       <c r="M21"/>
     </row>
     <row r="22" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2077,14 +2005,14 @@
       <c r="F22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="20"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K22" s="51" t="s">
+      <c r="K22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="20"/>
+      <c r="L22" s="16"/>
       <c r="M22"/>
     </row>
     <row r="23" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2106,8 +2034,8 @@
       <c r="F23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="G23" s="16"/>
+      <c r="L23" s="16"/>
       <c r="M23"/>
     </row>
     <row r="24" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2126,9 +2054,8 @@
       <c r="E24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="20"/>
+      <c r="G24" s="16"/>
+      <c r="L24" s="16"/>
       <c r="M24"/>
     </row>
     <row r="25" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -2150,9 +2077,8 @@
       <c r="F25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="20"/>
+      <c r="G25" s="16"/>
+      <c r="L25" s="16"/>
       <c r="M25"/>
     </row>
     <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2174,39 +2100,37 @@
       <c r="F26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="20"/>
+      <c r="G26" s="16"/>
       <c r="H26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K26" s="51"/>
-      <c r="L26" s="20"/>
+      <c r="L26" s="16"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="46" t="s">
+    <row r="27" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B27" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="46" t="s">
+      <c r="B27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D27" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" s="46" t="s">
+      <c r="D27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="46" t="s">
+      <c r="G27" s="16"/>
+      <c r="H27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="51"/>
-      <c r="L27" s="27"/>
+      <c r="L27" s="16"/>
       <c r="M27"/>
     </row>
     <row r="28" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2228,9 +2152,8 @@
       <c r="F28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="20"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="20"/>
+      <c r="G28" s="16"/>
+      <c r="L28" s="16"/>
       <c r="M28"/>
     </row>
     <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2252,65 +2175,57 @@
       <c r="F29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="20"/>
+      <c r="G29" s="16"/>
       <c r="H29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="51"/>
-      <c r="L29" s="20"/>
+      <c r="L29" s="16"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B30" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="28" t="s">
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D30" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="28" t="s">
+      <c r="D30" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="27"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="27"/>
+      <c r="G30" s="16"/>
+      <c r="L30" s="16"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D31" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="30" t="s">
+      <c r="D31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="27"/>
+      <c r="G31" s="16"/>
+      <c r="L31" s="16"/>
       <c r="M31"/>
     </row>
     <row r="32" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2332,11 +2247,8 @@
       <c r="F32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="20"/>
+      <c r="G32" s="16"/>
+      <c r="L32" s="16"/>
       <c r="M32"/>
     </row>
     <row r="33" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2358,9 +2270,8 @@
       <c r="F33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="20"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="20"/>
+      <c r="G33" s="16"/>
+      <c r="L33" s="16"/>
       <c r="M33"/>
     </row>
     <row r="34" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2382,33 +2293,31 @@
       <c r="F34" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="G34" s="20"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="20"/>
+      <c r="G34" s="16"/>
+      <c r="L34" s="16"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="1:13" s="36" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A35" s="36" t="s">
+    <row r="35" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D35" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="36" t="s">
+      <c r="D35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="G35" s="27"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="27"/>
+      <c r="G35" s="16"/>
+      <c r="L35" s="16"/>
     </row>
     <row r="36" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
@@ -2429,55 +2338,53 @@
       <c r="F36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="20"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="20"/>
+      <c r="G36" s="16"/>
+      <c r="L36" s="16"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="38" t="s">
+    <row r="37" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="B37" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="38" t="s">
+      <c r="B37" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="D37" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="38" t="s">
+      <c r="D37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="39"/>
-      <c r="L37" s="39"/>
-    </row>
-    <row r="38" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="48" t="s">
+      <c r="G37" s="22"/>
+      <c r="L37" s="22"/>
+    </row>
+    <row r="38" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B38" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="48" t="s">
+      <c r="B38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D38" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="48" t="s">
+      <c r="D38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="27"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="27"/>
+      <c r="G38" s="16"/>
+      <c r="L38" s="16"/>
     </row>
     <row r="39" spans="1:13" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
@@ -2498,9 +2405,8 @@
       <c r="F39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="20"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="20"/>
+      <c r="G39" s="16"/>
+      <c r="L39" s="16"/>
       <c r="M39"/>
     </row>
     <row r="40" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2522,9 +2428,8 @@
       <c r="F40" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="20"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="20"/>
+      <c r="G40" s="16"/>
+      <c r="L40" s="16"/>
       <c r="M40"/>
     </row>
     <row r="41" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2546,36 +2451,31 @@
       <c r="F41" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="20"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="20"/>
+      <c r="G41" s="16"/>
+      <c r="L41" s="16"/>
       <c r="M41"/>
     </row>
-    <row r="42" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="30" t="s">
+    <row r="42" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D42" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="30" t="s">
+      <c r="D42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="G42" s="27"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="27"/>
+      <c r="G42" s="16"/>
+      <c r="L42" s="16"/>
       <c r="M42"/>
     </row>
     <row r="43" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2597,11 +2497,8 @@
       <c r="F43" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="20"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="20"/>
+      <c r="G43" s="16"/>
+      <c r="L43" s="16"/>
       <c r="M43"/>
     </row>
     <row r="44" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2623,8 +2520,8 @@
       <c r="F44" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G44" s="20"/>
-      <c r="L44" s="20"/>
+      <c r="G44" s="16"/>
+      <c r="L44" s="16"/>
       <c r="M44"/>
     </row>
     <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -2646,21 +2543,21 @@
       <c r="F45" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="G45" s="20"/>
-      <c r="L45" s="20"/>
+      <c r="G45" s="16"/>
+      <c r="L45" s="16"/>
       <c r="M45"/>
     </row>
     <row r="46" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="52" t="s">
+      <c r="A46" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="52" t="s">
+      <c r="B46" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="52" t="b">
+      <c r="D46" s="23" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
@@ -2669,19 +2566,17 @@
       <c r="F46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="20"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="20"/>
+      <c r="G46" s="16"/>
+      <c r="L46" s="16"/>
       <c r="M46"/>
     </row>
     <row r="47" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="52"/>
-      <c r="B47" s="52"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="G47" s="20"/>
-      <c r="K47" s="51"/>
-      <c r="L47" s="20"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="G47" s="16"/>
+      <c r="L47" s="16"/>
       <c r="M47"/>
     </row>
     <row r="48" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2700,9 +2595,8 @@
       <c r="E48" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G48" s="20"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="20"/>
+      <c r="G48" s="16"/>
+      <c r="L48" s="16"/>
       <c r="M48"/>
     </row>
     <row r="49" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2721,9 +2615,8 @@
       <c r="E49" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G49" s="20"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="20"/>
+      <c r="G49" s="16"/>
+      <c r="L49" s="16"/>
       <c r="M49"/>
     </row>
     <row r="50" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2745,9 +2638,8 @@
       <c r="F50" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="G50" s="21"/>
-      <c r="K50" s="51"/>
-      <c r="L50" s="21"/>
+      <c r="G50" s="17"/>
+      <c r="L50" s="17"/>
       <c r="M50"/>
     </row>
     <row r="51" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2762,15 +2654,8 @@
       <c r="E51" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F51" s="50" t="s">
-        <v>309</v>
-      </c>
-      <c r="G51" s="21"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="51"/>
-      <c r="L51" s="21"/>
+      <c r="G51" s="17"/>
+      <c r="L51" s="17"/>
       <c r="M51"/>
     </row>
     <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -2792,8 +2677,8 @@
       <c r="F52" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="20"/>
-      <c r="L52" s="20"/>
+      <c r="G52" s="16"/>
+      <c r="L52" s="16"/>
       <c r="M52"/>
     </row>
     <row r="53" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2815,8 +2700,8 @@
       <c r="F53" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="G53" s="20"/>
-      <c r="L53" s="20"/>
+      <c r="G53" s="16"/>
+      <c r="L53" s="16"/>
       <c r="M53"/>
     </row>
     <row r="54" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2838,9 +2723,8 @@
       <c r="F54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G54" s="20"/>
-      <c r="K54" s="51"/>
-      <c r="L54" s="20"/>
+      <c r="G54" s="16"/>
+      <c r="L54" s="16"/>
       <c r="M54"/>
     </row>
     <row r="55" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2862,9 +2746,8 @@
       <c r="F55" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G55" s="20"/>
-      <c r="K55" s="51"/>
-      <c r="L55" s="20"/>
+      <c r="G55" s="16"/>
+      <c r="L55" s="16"/>
       <c r="M55"/>
     </row>
     <row r="56" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -2886,8 +2769,8 @@
       <c r="F56" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G56" s="20"/>
-      <c r="L56" s="20"/>
+      <c r="G56" s="16"/>
+      <c r="L56" s="16"/>
       <c r="M56"/>
     </row>
     <row r="57" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2909,61 +2792,59 @@
       <c r="F57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G57" s="20"/>
-      <c r="K57" s="51"/>
-      <c r="L57" s="20"/>
+      <c r="G57" s="16"/>
+      <c r="L57" s="16"/>
       <c r="M57"/>
     </row>
-    <row r="58" spans="1:13" s="47" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="47" t="s">
+    <row r="58" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B58" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="47" t="s">
+      <c r="B58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D58" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="47" t="s">
+      <c r="D58" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="27"/>
-      <c r="H58" s="47" t="s">
+      <c r="G58" s="16"/>
+      <c r="H58" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K58" s="51"/>
-      <c r="L58" s="27"/>
+      <c r="L58" s="16"/>
       <c r="M58"/>
     </row>
     <row r="59" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="D59" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="16"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="22"/>
+      <c r="D59" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="13"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="18"/>
       <c r="M59"/>
     </row>
     <row r="60" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -2985,8 +2866,8 @@
       <c r="F60" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="G60" s="27"/>
-      <c r="L60" s="27"/>
+      <c r="G60" s="16"/>
+      <c r="L60" s="16"/>
     </row>
     <row r="61" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
@@ -3004,13 +2885,13 @@
       <c r="E61" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F61" s="33"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="33"/>
-      <c r="L61" s="27"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="16"/>
     </row>
     <row r="62" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
@@ -3028,35 +2909,35 @@
       <c r="E62" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G62" s="20"/>
-      <c r="L62" s="20"/>
+      <c r="G62" s="16"/>
+      <c r="L62" s="16"/>
       <c r="M62"/>
     </row>
     <row r="63" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="D63" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="16" t="s">
+      <c r="D63" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="G63" s="22"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="22"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="18"/>
       <c r="M63"/>
     </row>
     <row r="64" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3078,11 +2959,11 @@
       <c r="F64" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G64" s="20"/>
-      <c r="L64" s="20"/>
+      <c r="G64" s="16"/>
+      <c r="L64" s="16"/>
       <c r="M64"/>
     </row>
-    <row r="65" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -3101,12 +2982,11 @@
       <c r="F65" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G65" s="20"/>
-      <c r="K65" s="51"/>
-      <c r="L65" s="20"/>
+      <c r="G65" s="16"/>
+      <c r="L65" s="16"/>
       <c r="M65"/>
     </row>
-    <row r="66" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
         <v>65</v>
       </c>
@@ -3125,11 +3005,11 @@
       <c r="F66" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="G66" s="20"/>
-      <c r="L66" s="20"/>
+      <c r="G66" s="16"/>
+      <c r="L66" s="16"/>
       <c r="M66"/>
     </row>
-    <row r="67" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>261</v>
       </c>
@@ -3148,11 +3028,11 @@
       <c r="F67" t="s">
         <v>226</v>
       </c>
-      <c r="G67" s="27"/>
-      <c r="L67" s="27"/>
+      <c r="G67" s="16"/>
+      <c r="L67" s="16"/>
       <c r="M67"/>
     </row>
-    <row r="68" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -3171,12 +3051,11 @@
       <c r="F68" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="G68" s="20"/>
-      <c r="K68" s="51"/>
-      <c r="L68" s="20"/>
+      <c r="G68" s="16"/>
+      <c r="L68" s="16"/>
       <c r="M68"/>
     </row>
-    <row r="69" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
@@ -3195,12 +3074,11 @@
       <c r="F69" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G69" s="20"/>
-      <c r="K69" s="51"/>
-      <c r="L69" s="20"/>
+      <c r="G69" s="16"/>
+      <c r="L69" s="16"/>
       <c r="M69"/>
     </row>
-    <row r="70" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>191</v>
       </c>
@@ -3219,36 +3097,34 @@
       <c r="F70" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G70" s="20"/>
-      <c r="K70" s="51"/>
-      <c r="L70" s="20"/>
+      <c r="G70" s="16"/>
+      <c r="L70" s="16"/>
       <c r="M70"/>
     </row>
-    <row r="71" spans="1:13" s="24" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="24" t="s">
+    <row r="71" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B71" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="24" t="s">
+      <c r="B71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D71" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="24" t="s">
+      <c r="D71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="G71" s="20"/>
-      <c r="K71" s="51"/>
-      <c r="L71" s="20"/>
+      <c r="G71" s="16"/>
+      <c r="L71" s="16"/>
       <c r="M71"/>
     </row>
-    <row r="72" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>72</v>
       </c>
@@ -3264,602 +3140,566 @@
       <c r="E72" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F72" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G72" s="20"/>
-      <c r="H72" s="43"/>
-      <c r="I72" s="43"/>
-      <c r="J72" s="43"/>
-      <c r="K72" s="51"/>
-      <c r="L72" s="21"/>
+      <c r="G72" s="16"/>
+      <c r="L72" s="17"/>
       <c r="M72"/>
     </row>
-    <row r="73" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="42" t="s">
+    <row r="73" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G73" s="16"/>
+      <c r="L73" s="16"/>
+      <c r="T73"/>
+    </row>
+    <row r="74" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D74" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G74" s="16"/>
+      <c r="L74" s="16"/>
+      <c r="T74"/>
+    </row>
+    <row r="75" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A75" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G75" s="16"/>
+      <c r="L75" s="16"/>
+      <c r="T75"/>
+    </row>
+    <row r="76" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G76" s="16"/>
+      <c r="L76" s="16"/>
+      <c r="T76"/>
+    </row>
+    <row r="77" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B77" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C73" s="42" t="s">
+      <c r="C77" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D73" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="42"/>
-      <c r="G73" s="20"/>
-      <c r="K73" s="51"/>
-      <c r="L73" s="20"/>
-      <c r="M73"/>
-    </row>
-    <row r="74" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="48" t="s">
+      <c r="D77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="16"/>
+      <c r="L77" s="16"/>
+      <c r="M77"/>
+    </row>
+    <row r="78" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B74" s="48" t="s">
+      <c r="B78" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="48" t="s">
+      <c r="C78" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D74" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="48" t="s">
+      <c r="D78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G74" s="27"/>
-      <c r="K74" s="51"/>
-      <c r="L74" s="27"/>
-      <c r="M74"/>
-    </row>
-    <row r="75" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="7" t="s">
+      <c r="G78" s="16"/>
+      <c r="L78" s="16"/>
+      <c r="M78"/>
+    </row>
+    <row r="79" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="7" t="s">
+      <c r="B79" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D75" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="7" t="s">
+      <c r="D79" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G75" s="20"/>
-      <c r="L75" s="20"/>
-      <c r="M75"/>
-    </row>
-    <row r="76" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="38" t="s">
+      <c r="G79" s="16"/>
+      <c r="L79" s="16"/>
+      <c r="M79"/>
+    </row>
+    <row r="80" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A80" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="B76" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="38" t="s">
+      <c r="B80" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="D76" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="45" t="s">
+      <c r="D80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G76" s="27"/>
-      <c r="L76" s="27"/>
-    </row>
-    <row r="77" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="2" t="s">
+      <c r="G80" s="16"/>
+      <c r="L80" s="16"/>
+    </row>
+    <row r="81" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="2" t="s">
+      <c r="B81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D77" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" s="2" t="s">
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G77" s="20"/>
-      <c r="K77" s="51"/>
-      <c r="L77" s="20"/>
-      <c r="M77"/>
-    </row>
-    <row r="78" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G78" s="20"/>
-      <c r="K78" s="51"/>
-      <c r="L78" s="20"/>
-      <c r="M78"/>
-    </row>
-    <row r="79" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D79" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="50" t="s">
-        <v>309</v>
-      </c>
-      <c r="G79" s="20"/>
-      <c r="H79" s="43"/>
-      <c r="I79" s="43"/>
-      <c r="J79" s="43"/>
-      <c r="K79" s="51"/>
-      <c r="L79" s="21"/>
-      <c r="M79"/>
-    </row>
-    <row r="80" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="G80" s="20"/>
-      <c r="K80" s="51"/>
-      <c r="L80" s="20"/>
-      <c r="M80"/>
-    </row>
-    <row r="81" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D81" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="G81" s="20"/>
-      <c r="L81" s="20"/>
+      <c r="G81" s="16"/>
+      <c r="L81" s="16"/>
       <c r="M81"/>
     </row>
     <row r="82" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G82" s="16"/>
+      <c r="L82" s="16"/>
+      <c r="M82"/>
+    </row>
+    <row r="83" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G83" s="16"/>
+      <c r="L83" s="17"/>
+      <c r="M83"/>
+    </row>
+    <row r="84" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G84" s="16"/>
+      <c r="L84" s="16"/>
+      <c r="M84"/>
+    </row>
+    <row r="85" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D85" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="G85" s="16"/>
+      <c r="L85" s="16"/>
+      <c r="M85"/>
+    </row>
+    <row r="86" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="2" t="s">
+      <c r="D86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G82" s="20"/>
-      <c r="K82" s="51"/>
-      <c r="L82" s="20"/>
-      <c r="M82"/>
-    </row>
-    <row r="83" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A83" s="7" t="s">
+      <c r="G86" s="16"/>
+      <c r="L86" s="16"/>
+      <c r="M86"/>
+    </row>
+    <row r="87" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A87" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B87" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C87" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D83" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="7" t="s">
+      <c r="D87" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="G83" s="20"/>
-      <c r="L83" s="20"/>
-      <c r="M83"/>
-    </row>
-    <row r="84" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
+      <c r="G87" s="16"/>
+      <c r="L87" s="16"/>
+      <c r="M87"/>
+    </row>
+    <row r="88" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="G84" s="20"/>
-      <c r="J84" s="17"/>
-      <c r="K84" s="51"/>
-      <c r="L84" s="20"/>
-      <c r="M84"/>
-    </row>
-    <row r="85" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
+      <c r="D88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="G88" s="16"/>
+      <c r="L88" s="16"/>
+      <c r="M88"/>
+    </row>
+    <row r="89" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="2" t="s">
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G85" s="20"/>
-      <c r="K85" s="51"/>
-      <c r="L85" s="20"/>
-      <c r="M85"/>
-    </row>
-    <row r="86" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="7" t="s">
+      <c r="G89" s="16"/>
+      <c r="L89" s="16"/>
+      <c r="M89"/>
+    </row>
+    <row r="90" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B90" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C90" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D86" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="7" t="s">
+      <c r="D90" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G86" s="20"/>
-      <c r="L86" s="20"/>
-      <c r="M86"/>
-    </row>
-    <row r="87" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="7" t="s">
+      <c r="G90" s="16"/>
+      <c r="L90" s="16"/>
+      <c r="M90"/>
+    </row>
+    <row r="91" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="7" t="s">
+      <c r="B91" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D87" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" s="7" t="s">
+      <c r="D91" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G87" s="20"/>
-      <c r="L87" s="20"/>
-      <c r="M87"/>
-    </row>
-    <row r="88" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="38" t="s">
+      <c r="G91" s="16"/>
+      <c r="L91" s="16"/>
+      <c r="M91"/>
+    </row>
+    <row r="92" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="B88" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="D88" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="38" t="s">
+      <c r="D92" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G88" s="39"/>
-      <c r="H88" s="38"/>
-      <c r="I88" s="38"/>
-      <c r="J88" s="38"/>
-      <c r="K88" s="38" t="s">
+      <c r="G92" s="22"/>
+      <c r="H92" s="21"/>
+      <c r="I92" s="21"/>
+      <c r="J92" s="21"/>
+      <c r="K92" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L88" s="27"/>
-      <c r="M88"/>
-    </row>
-    <row r="89" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
+      <c r="L92" s="16"/>
+      <c r="M92"/>
+    </row>
+    <row r="93" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" s="2" t="s">
+      <c r="D93" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G89" s="20"/>
-      <c r="K89" s="51"/>
-      <c r="L89" s="20"/>
-      <c r="M89"/>
-    </row>
-    <row r="90" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
+      <c r="G93" s="16"/>
+      <c r="L93" s="16"/>
+      <c r="M93"/>
+    </row>
+    <row r="94" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="2" t="s">
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G90" s="20"/>
-      <c r="J90" s="2" t="s">
+      <c r="G94" s="16"/>
+      <c r="J94" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K90" s="51"/>
-      <c r="L90" s="20"/>
-      <c r="M90"/>
-    </row>
-    <row r="91" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
+      <c r="L94" s="16"/>
+      <c r="M94"/>
+    </row>
+    <row r="95" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
+      <c r="B95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="2" t="s">
+      <c r="D95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G91" s="20"/>
-      <c r="K91" s="51"/>
-      <c r="L91" s="20"/>
-      <c r="M91"/>
-    </row>
-    <row r="92" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B92" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C92" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D92" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F92" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="G92" s="27"/>
-      <c r="K92" s="51"/>
-      <c r="L92" s="27"/>
-      <c r="M92"/>
-    </row>
-    <row r="93" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="G93" s="20"/>
-      <c r="K93" s="51"/>
-      <c r="L93" s="20"/>
-      <c r="M93"/>
-    </row>
-    <row r="94" spans="1:13" s="49" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="49" t="s">
-        <v>303</v>
-      </c>
-      <c r="B94" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="49" t="s">
-        <v>304</v>
-      </c>
-      <c r="D94" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="G94" s="27"/>
-      <c r="H94" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="K94" s="51"/>
-      <c r="L94" s="27"/>
-      <c r="M94"/>
-    </row>
-    <row r="95" spans="1:13" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A95" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="D95" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="G95" s="20"/>
-      <c r="K95" s="51"/>
-      <c r="L95" s="20"/>
+      <c r="G95" s="16"/>
+      <c r="L95" s="16"/>
       <c r="M95"/>
     </row>
     <row r="96" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B96" s="8"/>
-      <c r="C96" s="8"/>
+        <v>98</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="D96" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="G96" s="20"/>
-      <c r="I96" s="34"/>
-      <c r="J96" s="34"/>
-      <c r="K96" s="51"/>
-      <c r="L96" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G96" s="16"/>
+      <c r="L96" s="16"/>
       <c r="M96"/>
     </row>
-    <row r="97" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>5</v>
+        <v>201</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="D97" s="2" t="b">
         <v>0</v>
@@ -3868,44 +3708,47 @@
         <v>1</v>
       </c>
       <c r="F97" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G97" s="16"/>
+      <c r="L97" s="16"/>
+      <c r="M97"/>
+    </row>
+    <row r="98" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G98" s="16"/>
+      <c r="H98" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G97" s="20"/>
-      <c r="K97" s="51"/>
-      <c r="L97" s="20"/>
-      <c r="M97"/>
-    </row>
-    <row r="98" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" t="s">
-        <v>276</v>
-      </c>
-      <c r="B98" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" t="s">
-        <v>277</v>
-      </c>
-      <c r="D98" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" t="s">
-        <v>305</v>
-      </c>
-      <c r="G98" s="27"/>
-      <c r="L98" s="27"/>
+      <c r="L98" s="16"/>
+      <c r="M98"/>
     </row>
     <row r="99" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>102</v>
+        <v>247</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>55</v>
+        <v>248</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>103</v>
+        <v>249</v>
       </c>
       <c r="D99" s="2" t="b">
         <v>0</v>
@@ -3914,340 +3757,312 @@
         <v>1</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="G99" s="20"/>
-      <c r="K99" s="51"/>
-      <c r="L99" s="20"/>
+        <v>250</v>
+      </c>
+      <c r="G99" s="16"/>
+      <c r="L99" s="16"/>
       <c r="M99"/>
     </row>
-    <row r="100" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>105</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
       <c r="D100" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G100" s="16"/>
+      <c r="L100" s="16"/>
+      <c r="M100"/>
+    </row>
+    <row r="101" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G100" s="20"/>
-      <c r="K100" s="51"/>
-      <c r="L100" s="20"/>
-      <c r="M100"/>
-    </row>
-    <row r="101" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G101" s="20"/>
-      <c r="K101" s="51"/>
-      <c r="L101" s="20"/>
+      <c r="G101" s="16"/>
+      <c r="L101" s="16"/>
       <c r="M101"/>
     </row>
-    <row r="102" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G102" s="20"/>
-      <c r="K102" s="51"/>
-      <c r="L102" s="20"/>
-      <c r="M102"/>
+    <row r="102" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
+        <v>276</v>
+      </c>
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" t="s">
+        <v>277</v>
+      </c>
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" t="s">
+        <v>305</v>
+      </c>
+      <c r="G102" s="16"/>
+      <c r="L102" s="16"/>
     </row>
     <row r="103" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="G103" s="16"/>
+      <c r="L103" s="16"/>
+      <c r="M103"/>
+    </row>
+    <row r="104" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A104" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D104" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" s="16"/>
+      <c r="L104" s="16"/>
+      <c r="M104"/>
+    </row>
+    <row r="105" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D105" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G105" s="16"/>
+      <c r="L105" s="16"/>
+      <c r="M105"/>
+    </row>
+    <row r="106" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G106" s="16"/>
+      <c r="L106" s="16"/>
+      <c r="M106"/>
+    </row>
+    <row r="107" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A107" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D103" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G103" s="20"/>
-      <c r="H103" s="43"/>
-      <c r="I103" s="43"/>
-      <c r="J103" s="43"/>
-      <c r="K103" s="51"/>
-      <c r="L103" s="21"/>
-      <c r="M103"/>
-    </row>
-    <row r="104" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="7" t="s">
+      <c r="D107" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G107" s="16"/>
+      <c r="L107" s="17"/>
+      <c r="M107"/>
+    </row>
+    <row r="108" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="B108" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C108" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D104" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" s="7" t="s">
+      <c r="D108" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="G104" s="20"/>
-      <c r="L104" s="20"/>
-      <c r="M104"/>
-    </row>
-    <row r="105" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="7" t="s">
+      <c r="G108" s="16"/>
+      <c r="L108" s="16"/>
+      <c r="M108"/>
+    </row>
+    <row r="109" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B109" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C109" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D105" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F105" s="7" t="s">
+      <c r="D109" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F109" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="G105" s="20"/>
-      <c r="L105" s="20"/>
-      <c r="M105"/>
-    </row>
-    <row r="106" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="7" t="s">
+      <c r="G109" s="16"/>
+      <c r="L109" s="16"/>
+      <c r="M109"/>
+    </row>
+    <row r="110" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B106" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" s="7" t="s">
+      <c r="B110" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D106" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F106" s="7" t="s">
+      <c r="D110" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G106" s="20"/>
-      <c r="L106" s="20"/>
-      <c r="M106"/>
-    </row>
-    <row r="107" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
+      <c r="G110" s="16"/>
+      <c r="L110" s="16"/>
+      <c r="M110"/>
+    </row>
+    <row r="111" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
+      <c r="B111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D107" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F107" s="2" t="s">
+      <c r="D111" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G107" s="20"/>
-      <c r="K107" s="51"/>
-      <c r="L107" s="20"/>
-      <c r="M107"/>
-    </row>
-    <row r="108" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="2" t="s">
+      <c r="G111" s="16"/>
+      <c r="L111" s="16"/>
+      <c r="M111"/>
+    </row>
+    <row r="112" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" s="2" t="s">
+      <c r="B112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D108" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F108" s="2" t="s">
+      <c r="D112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G108" s="20"/>
-      <c r="K108" s="51"/>
-      <c r="L108" s="20"/>
-      <c r="M108"/>
-    </row>
-    <row r="109" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D109" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G109" s="20"/>
-      <c r="H109" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K109" s="51"/>
-      <c r="L109" s="20"/>
-      <c r="M109"/>
-    </row>
-    <row r="110" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A110" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D110" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E110" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G110" s="20"/>
-      <c r="H110"/>
-      <c r="I110"/>
-      <c r="J110"/>
-      <c r="K110"/>
-      <c r="L110" s="20"/>
-      <c r="M110"/>
-    </row>
-    <row r="111" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>278</v>
-      </c>
-      <c r="B111" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" t="s">
-        <v>279</v>
-      </c>
-      <c r="D111" t="b">
-        <v>0</v>
-      </c>
-      <c r="E111" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" t="s">
-        <v>4</v>
-      </c>
-      <c r="G111" s="27"/>
-      <c r="H111"/>
-      <c r="I111"/>
-      <c r="J111"/>
-      <c r="K111"/>
-      <c r="L111" s="27"/>
-    </row>
-    <row r="112" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A112" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D112" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G112" s="20"/>
-      <c r="L112" s="20"/>
+      <c r="G112" s="16"/>
+      <c r="L112" s="16"/>
+      <c r="M112"/>
     </row>
     <row r="113" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D113" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E113" s="2" t="b">
         <v>1</v>
@@ -4255,25 +4070,25 @@
       <c r="F113" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G113" s="20"/>
+      <c r="G113" s="16"/>
       <c r="H113" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K113" s="51"/>
-      <c r="L113" s="20"/>
-    </row>
-    <row r="114" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="L113" s="16"/>
+      <c r="M113"/>
+    </row>
+    <row r="114" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
-        <v>238</v>
+        <v>152</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="D114" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E114" s="2" t="b">
         <v>1</v>
@@ -4281,119 +4096,196 @@
       <c r="F114" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G114" s="20"/>
-      <c r="H114" s="2" t="s">
+      <c r="G114" s="16"/>
+      <c r="H114"/>
+      <c r="I114"/>
+      <c r="J114"/>
+      <c r="K114"/>
+      <c r="L114" s="16"/>
+      <c r="M114"/>
+    </row>
+    <row r="115" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A115" t="s">
+        <v>278</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" t="s">
+        <v>279</v>
+      </c>
+      <c r="D115" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" t="s">
+        <v>4</v>
+      </c>
+      <c r="G115" s="16"/>
+      <c r="H115"/>
+      <c r="I115"/>
+      <c r="J115"/>
+      <c r="K115"/>
+      <c r="L115" s="16"/>
+    </row>
+    <row r="116" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A116" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D116" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F116" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K114" s="51"/>
-      <c r="L114" s="20"/>
-    </row>
-    <row r="115" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="2" t="s">
+      <c r="G116" s="16"/>
+      <c r="L116" s="16"/>
+    </row>
+    <row r="117" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D117" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G117" s="16"/>
+      <c r="H117" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L117" s="16"/>
+    </row>
+    <row r="118" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D118" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G118" s="16"/>
+      <c r="H118" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L118" s="16"/>
+    </row>
+    <row r="119" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D115" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F115" s="43" t="s">
+      <c r="D119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="G115" s="20"/>
-      <c r="K115" s="51"/>
-      <c r="L115" s="20"/>
-    </row>
-    <row r="116" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A116" s="44" t="s">
+      <c r="G119" s="16"/>
+      <c r="L119" s="16"/>
+    </row>
+    <row r="120" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B116" s="44" t="s">
+      <c r="B120" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C116" s="44" t="s">
+      <c r="C120" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D116" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" s="50" t="s">
-        <v>309</v>
-      </c>
-      <c r="G116" s="27"/>
-      <c r="K116" s="51"/>
-      <c r="L116" s="21"/>
-    </row>
-    <row r="117" spans="1:13" s="25" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A117" s="26" t="s">
+      <c r="D120" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G120" s="16"/>
+      <c r="L120" s="17"/>
+    </row>
+    <row r="121" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A121" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B117" s="26" t="s">
+      <c r="B121" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C117" s="26" t="s">
+      <c r="C121" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D117" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F117" s="26" t="s">
+      <c r="D121" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="G117" s="27"/>
-      <c r="H117" s="26"/>
-      <c r="I117" s="26"/>
-      <c r="J117" s="26"/>
-      <c r="K117" s="51"/>
-      <c r="L117" s="27"/>
-    </row>
-    <row r="118" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A118" s="2" t="s">
+      <c r="G121" s="16"/>
+      <c r="L121" s="16"/>
+    </row>
+    <row r="122" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A122" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D118" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E118" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F118" s="2" t="s">
+      <c r="D122" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G118" s="20"/>
-      <c r="K118" s="51"/>
-      <c r="L118" s="20"/>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="M119"/>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="M120"/>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="M121"/>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="M122"/>
+      <c r="G122" s="16"/>
+      <c r="L122" s="16"/>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.4">
       <c r="M123"/>
@@ -4448,6 +4340,18 @@
     </row>
     <row r="140" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M140"/>
+    </row>
+    <row r="141" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M141"/>
+    </row>
+    <row r="142" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M142"/>
+    </row>
+    <row r="143" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M143"/>
+    </row>
+    <row r="144" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M144"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4461,8 +4365,8 @@
     <mergeCell ref="D46:D47"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1"/>
-    <hyperlink ref="F21" r:id="rId2"/>
+    <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId3"/>
@@ -4470,7 +4374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
BIJ12: Standaard wordt documentatie via Documentor gegenereerd.
Minor, configuratie.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BIJ12/props/BIJ12.xlsx
+++ b/src/main/resources/input/BIJ12/props/BIJ12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\BIJ12\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2236A2CA-6C2F-4067-866E-E698D00F5859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6058BF49-7963-4205-BEB9-2F2AB9BEDA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BIJ12" sheetId="3" r:id="rId1"/>
@@ -841,15 +841,9 @@
     <t>createofficevariant</t>
   </si>
   <si>
-    <t>respec/msword</t>
-  </si>
-  <si>
     <t>Specify the type of office file. Multiple formats are allowed, separate list by whitespace.</t>
   </si>
   <si>
-    <t>respec</t>
-  </si>
-  <si>
     <t>createskos</t>
   </si>
   <si>
@@ -1007,6 +1001,12 @@
   </si>
   <si>
     <t>1.1</t>
+  </si>
+  <si>
+    <t>respec/msword/documentor</t>
+  </si>
+  <si>
+    <t>documentor</t>
   </si>
 </sst>
 </file>
@@ -1502,10 +1502,10 @@
   <dimension ref="A1:T144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G74" sqref="G74"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1565,16 +1565,16 @@
       <c r="F2" s="3"/>
       <c r="G2" s="15"/>
       <c r="H2" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="L2" s="15"/>
       <c r="M2" s="5"/>
@@ -1914,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G18" s="16"/>
       <c r="L18" s="16"/>
@@ -1957,7 +1957,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G20" s="16"/>
       <c r="L20" s="16"/>
@@ -1980,7 +1980,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G21" s="16"/>
       <c r="L21" s="16"/>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="27" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
@@ -2222,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G31" s="16"/>
       <c r="L31" s="16"/>
@@ -2302,11 +2302,11 @@
         <v>270</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>272</v>
-      </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>273</v>
+        <v>326</v>
       </c>
       <c r="G35" s="16"/>
       <c r="L35" s="16"/>
@@ -2344,13 +2344,13 @@
     </row>
     <row r="37" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="21" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D37" s="21" t="b">
         <v>0</v>
@@ -2366,13 +2366,13 @@
     </row>
     <row r="38" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D38" s="2" t="b">
         <v>0</v>
@@ -2472,7 +2472,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G42" s="16"/>
       <c r="L42" s="16"/>
@@ -2798,13 +2798,13 @@
     </row>
     <row r="58" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D58" s="2" t="b">
         <v>0</v>
@@ -2824,13 +2824,13 @@
     </row>
     <row r="59" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A59" s="13" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D59" s="13" t="b">
         <v>0</v>
@@ -2849,35 +2849,35 @@
     </row>
     <row r="60" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>285</v>
       </c>
       <c r="G60" s="16"/>
       <c r="L60" s="16"/>
     </row>
     <row r="61" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D61" s="7" t="b">
         <v>0</v>
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G69" s="16"/>
       <c r="L69" s="16"/>
@@ -3146,13 +3146,13 @@
     </row>
     <row r="73" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>0</v>
@@ -3161,7 +3161,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G73" s="16"/>
       <c r="L73" s="16"/>
@@ -3169,13 +3169,13 @@
     </row>
     <row r="74" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>240</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
@@ -3184,7 +3184,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G74" s="16"/>
       <c r="L74" s="16"/>
@@ -3192,13 +3192,13 @@
     </row>
     <row r="75" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -3207,7 +3207,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G75" s="16"/>
       <c r="L75" s="16"/>
@@ -3215,13 +3215,13 @@
     </row>
     <row r="76" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>240</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
@@ -3241,7 +3241,7 @@
         <v>10</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D77" s="2" t="b">
         <v>0</v>
@@ -3255,13 +3255,13 @@
     </row>
     <row r="78" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
@@ -3301,13 +3301,13 @@
     </row>
     <row r="80" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B80" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D80" s="2" t="b">
         <v>0</v>
@@ -3427,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G85" s="16"/>
       <c r="L85" s="16"/>
@@ -3496,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G88" s="16"/>
       <c r="L88" s="16"/>
@@ -3573,13 +3573,13 @@
     </row>
     <row r="92" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A92" s="21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B92" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D92" s="21" t="b">
         <v>0</v>
@@ -3716,13 +3716,13 @@
     </row>
     <row r="98" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D98" s="2" t="b">
         <v>0</v>
@@ -3776,7 +3776,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G100" s="16"/>
       <c r="L100" s="16"/>
@@ -3807,13 +3807,13 @@
     </row>
     <row r="102" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B102" t="s">
         <v>10</v>
       </c>
       <c r="C102" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D102" t="b">
         <v>1</v>
@@ -3822,7 +3822,7 @@
         <v>1</v>
       </c>
       <c r="F102" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G102" s="16"/>
       <c r="L102" s="16"/>
@@ -3844,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G103" s="16"/>
       <c r="L103" s="16"/>
@@ -4106,13 +4106,13 @@
     </row>
     <row r="115" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D115" t="b">
         <v>0</v>
@@ -4219,20 +4219,20 @@
         <v>0</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G119" s="16"/>
       <c r="L119" s="16"/>
     </row>
     <row r="120" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D120" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Referentie naar dashboardpath property verwijderd
Sinds eind 2024 is het dashboard niet meer actief. Daarmee is de relatie
tussen Imvertor en de Imvertor SaaS niet meer relevant en is dit zuiver
één richting gemaakt; Imvertor is SaaS agnostisch.

Improvement.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/BIJ12/props/BIJ12.xlsx
+++ b/src/main/resources/input/BIJ12/props/BIJ12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\BIJ12\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6058BF49-7963-4205-BEB9-2F2AB9BEDA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F85463-B5D0-4488-A027-5F351E08138C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BIJ12" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="324">
   <si>
     <t>Name</t>
   </si>
@@ -167,15 +167,6 @@
   </si>
   <si>
     <t>Yes if the released application should be zipped for distribution</t>
-  </si>
-  <si>
-    <t>dashboardpath</t>
-  </si>
-  <si>
-    <t>http-path</t>
-  </si>
-  <si>
-    <t>The path to the Imvertor dashboard application.</t>
   </si>
   <si>
     <t>debug</t>
@@ -1499,13 +1490,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T144"/>
+  <dimension ref="A1:T143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="E45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1535,59 +1526,59 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="56.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="15"/>
       <c r="H2" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>311</v>
       </c>
       <c r="L2" s="15"/>
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1647,13 +1638,13 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D6" s="7" t="b">
         <v>0</v>
@@ -1696,13 +1687,13 @@
     </row>
     <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D9" s="7" t="b">
         <v>0</v>
@@ -1742,13 +1733,13 @@
     </row>
     <row r="11" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>0</v>
@@ -1762,13 +1753,13 @@
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
@@ -1785,22 +1776,22 @@
     </row>
     <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="G13" s="16"/>
       <c r="L13" s="16"/>
@@ -1850,7 +1841,7 @@
       </c>
       <c r="G15" s="16"/>
       <c r="J15" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L15" s="16"/>
       <c r="M15"/>
@@ -1880,13 +1871,13 @@
     </row>
     <row r="17" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>1</v>
@@ -1895,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G17" s="16"/>
       <c r="L17" s="16"/>
@@ -1903,7 +1894,7 @@
     </row>
     <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1914,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G18" s="16"/>
       <c r="L18" s="16"/>
@@ -1922,13 +1913,13 @@
     </row>
     <row r="19" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
@@ -1942,13 +1933,13 @@
     </row>
     <row r="20" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
@@ -1957,7 +1948,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G20" s="16"/>
       <c r="L20" s="16"/>
@@ -1965,13 +1956,13 @@
     </row>
     <row r="21" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
@@ -1980,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G21" s="16"/>
       <c r="L21" s="16"/>
@@ -1988,13 +1979,13 @@
     </row>
     <row r="22" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
@@ -2040,13 +2031,13 @@
     </row>
     <row r="24" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>
@@ -2109,13 +2100,13 @@
     </row>
     <row r="27" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
@@ -2158,13 +2149,13 @@
     </row>
     <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D29" s="2" t="b">
         <v>0</v>
@@ -2184,13 +2175,13 @@
     </row>
     <row r="30" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D30" s="2" t="b">
         <v>0</v>
@@ -2207,13 +2198,13 @@
     </row>
     <row r="31" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D31" s="2" t="b">
         <v>0</v>
@@ -2222,7 +2213,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G31" s="16"/>
       <c r="L31" s="16"/>
@@ -2253,13 +2244,13 @@
     </row>
     <row r="33" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
@@ -2276,13 +2267,13 @@
     </row>
     <row r="34" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D34" s="2" t="b">
         <v>0</v>
@@ -2291,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G34" s="16"/>
       <c r="L34" s="16"/>
@@ -2299,13 +2290,13 @@
     </row>
     <row r="35" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
@@ -2314,7 +2305,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G35" s="16"/>
       <c r="L35" s="16"/>
@@ -2344,13 +2335,13 @@
     </row>
     <row r="37" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="21" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D37" s="21" t="b">
         <v>0</v>
@@ -2366,13 +2357,13 @@
     </row>
     <row r="38" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D38" s="2" t="b">
         <v>0</v>
@@ -2457,13 +2448,13 @@
     </row>
     <row r="42" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D42" s="2" t="b">
         <v>0</v>
@@ -2472,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G42" s="16"/>
       <c r="L42" s="16"/>
@@ -2480,13 +2471,13 @@
     </row>
     <row r="43" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D43" s="2" t="b">
         <v>0</v>
@@ -2524,87 +2515,84 @@
       <c r="L44" s="16"/>
       <c r="M44"/>
     </row>
-    <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>218</v>
+      <c r="D45" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G45" s="16"/>
       <c r="L45" s="16"/>
       <c r="M45"/>
     </row>
     <row r="46" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
       <c r="G46" s="16"/>
       <c r="L46" s="16"/>
       <c r="M46"/>
     </row>
-    <row r="47" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
+    <row r="47" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="G47" s="16"/>
       <c r="L47" s="16"/>
       <c r="M47"/>
     </row>
-    <row r="48" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>176</v>
+        <v>49</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>177</v>
+        <v>5</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>178</v>
+        <v>50</v>
       </c>
       <c r="D48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="16"/>
       <c r="L48" s="16"/>
       <c r="M48"/>
     </row>
-    <row r="49" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>53</v>
@@ -2615,55 +2603,58 @@
       <c r="E49" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G49" s="16"/>
-      <c r="L49" s="16"/>
+      <c r="F49" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="G49" s="17"/>
+      <c r="L49" s="17"/>
       <c r="M49"/>
     </row>
-    <row r="50" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
       <c r="D50" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="G50" s="17"/>
       <c r="L50" s="17"/>
       <c r="M50"/>
     </row>
-    <row r="51" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G51" s="17"/>
-      <c r="L51" s="17"/>
+    <row r="51" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D51" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="16"/>
+      <c r="L51" s="16"/>
       <c r="M51"/>
     </row>
-    <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>180</v>
@@ -2675,30 +2666,30 @@
         <v>1</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="G52" s="16"/>
       <c r="L52" s="16"/>
       <c r="M52"/>
     </row>
-    <row r="53" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A53" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D53" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>209</v>
+    <row r="53" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G53" s="16"/>
       <c r="L53" s="16"/>
@@ -2706,13 +2697,13 @@
     </row>
     <row r="54" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D54" s="2" t="b">
         <v>0</v>
@@ -2727,61 +2718,61 @@
       <c r="L54" s="16"/>
       <c r="M54"/>
     </row>
-    <row r="55" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="D55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="16"/>
       <c r="L55" s="16"/>
       <c r="M55"/>
     </row>
-    <row r="56" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D56" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F56" s="7" t="s">
+    <row r="56" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D56" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G56" s="16"/>
       <c r="L56" s="16"/>
       <c r="M56"/>
     </row>
-    <row r="57" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
-        <v>184</v>
+        <v>292</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>185</v>
+        <v>293</v>
       </c>
       <c r="D57" s="2" t="b">
         <v>0</v>
@@ -2790,69 +2781,68 @@
         <v>1</v>
       </c>
       <c r="F57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="16"/>
+      <c r="H57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G57" s="16"/>
       <c r="L57" s="16"/>
       <c r="M57"/>
     </row>
-    <row r="58" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G58" s="16"/>
-      <c r="H58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="16"/>
+    <row r="58" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A58" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D58" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="13"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="18"/>
       <c r="M58"/>
     </row>
-    <row r="59" spans="1:13" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A59" s="13" t="s">
+    <row r="59" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="B59" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="D59" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="13"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="18"/>
-      <c r="M59"/>
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="G59" s="16"/>
+      <c r="L59" s="16"/>
     </row>
     <row r="60" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>281</v>
+        <v>86</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>282</v>
@@ -2863,21 +2853,23 @@
       <c r="E60" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F60" s="7" t="s">
-        <v>283</v>
-      </c>
+      <c r="F60" s="20"/>
       <c r="G60" s="16"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
       <c r="L60" s="16"/>
     </row>
-    <row r="61" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
-        <v>284</v>
+        <v>183</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>285</v>
+        <v>184</v>
       </c>
       <c r="D61" s="7" t="b">
         <v>0</v>
@@ -2885,163 +2877,162 @@
       <c r="E61" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F61" s="20"/>
       <c r="G61" s="16"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
-      <c r="J61" s="20"/>
-      <c r="K61" s="20"/>
       <c r="L61" s="16"/>
-    </row>
-    <row r="62" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="7" t="s">
+      <c r="M61"/>
+    </row>
+    <row r="62" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D62" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="G62" s="18"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="18"/>
+      <c r="M62"/>
+    </row>
+    <row r="63" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C62" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G62" s="16"/>
-      <c r="L62" s="16"/>
-      <c r="M62"/>
-    </row>
-    <row r="63" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D63" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="G63" s="18"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="18"/>
+      <c r="D63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="16"/>
+      <c r="L63" s="16"/>
       <c r="M63"/>
     </row>
-    <row r="64" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>19</v>
+    <row r="64" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="G64" s="16"/>
       <c r="L64" s="16"/>
       <c r="M64"/>
     </row>
-    <row r="65" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>207</v>
+      <c r="D65" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="G65" s="16"/>
       <c r="L65" s="16"/>
       <c r="M65"/>
     </row>
     <row r="66" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D66" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>218</v>
+      <c r="A66" t="s">
+        <v>258</v>
+      </c>
+      <c r="B66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" t="s">
+        <v>259</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>223</v>
       </c>
       <c r="G66" s="16"/>
       <c r="L66" s="16"/>
       <c r="M66"/>
     </row>
-    <row r="67" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
-        <v>261</v>
-      </c>
-      <c r="B67" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" t="s">
-        <v>262</v>
-      </c>
-      <c r="D67" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" t="s">
-        <v>226</v>
+    <row r="67" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="G67" s="16"/>
       <c r="L67" s="16"/>
       <c r="M67"/>
     </row>
-    <row r="68" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
       </c>
@@ -3049,30 +3040,30 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>210</v>
+        <v>303</v>
       </c>
       <c r="G68" s="16"/>
       <c r="L68" s="16"/>
       <c r="M68"/>
     </row>
-    <row r="69" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>70</v>
+        <v>188</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>10</v>
+        <v>189</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E69" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>306</v>
+        <v>205</v>
       </c>
       <c r="G69" s="16"/>
       <c r="L69" s="16"/>
@@ -3080,13 +3071,13 @@
     </row>
     <row r="70" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>192</v>
+        <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>193</v>
+        <v>252</v>
       </c>
       <c r="D70" s="2" t="b">
         <v>0</v>
@@ -3095,61 +3086,61 @@
         <v>1</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>208</v>
+        <v>251</v>
       </c>
       <c r="G70" s="16"/>
       <c r="L70" s="16"/>
       <c r="M70"/>
     </row>
-    <row r="71" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>253</v>
+        <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>255</v>
+        <v>70</v>
       </c>
       <c r="D71" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>254</v>
+        <v>0</v>
       </c>
       <c r="G71" s="16"/>
-      <c r="L71" s="16"/>
+      <c r="L71" s="17"/>
       <c r="M71"/>
     </row>
-    <row r="72" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>72</v>
+        <v>311</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>73</v>
+        <v>312</v>
       </c>
       <c r="D72" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>313</v>
       </c>
       <c r="G72" s="16"/>
-      <c r="L72" s="17"/>
-      <c r="M72"/>
+      <c r="L72" s="16"/>
+      <c r="T72"/>
     </row>
     <row r="73" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>315</v>
@@ -3161,7 +3152,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="G73" s="16"/>
       <c r="L73" s="16"/>
@@ -3169,22 +3160,22 @@
     </row>
     <row r="74" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="D74" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>324</v>
       </c>
       <c r="G74" s="16"/>
       <c r="L74" s="16"/>
@@ -3195,7 +3186,7 @@
         <v>319</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>320</v>
@@ -3205,9 +3196,6 @@
       </c>
       <c r="E75" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="G75" s="16"/>
       <c r="L75" s="16"/>
@@ -3215,13 +3203,13 @@
     </row>
     <row r="76" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>322</v>
+        <v>191</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>240</v>
+        <v>10</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>323</v>
+        <v>284</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
@@ -3231,249 +3219,252 @@
       </c>
       <c r="G76" s="16"/>
       <c r="L76" s="16"/>
-      <c r="T76"/>
-    </row>
-    <row r="77" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="M76"/>
+    </row>
+    <row r="77" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>194</v>
+        <v>294</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="D77" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E77" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="G77" s="16"/>
       <c r="L77" s="16"/>
       <c r="M77"/>
     </row>
-    <row r="78" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="D78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>226</v>
+    <row r="78" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="G78" s="16"/>
       <c r="L78" s="16"/>
       <c r="M78"/>
     </row>
-    <row r="79" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>4</v>
+    <row r="79" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A79" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G79" s="16"/>
       <c r="L79" s="16"/>
-      <c r="M79"/>
-    </row>
-    <row r="80" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="B80" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="21" t="s">
-        <v>292</v>
+    </row>
+    <row r="80" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="D80" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G80" s="16"/>
       <c r="L80" s="16"/>
+      <c r="M80"/>
     </row>
     <row r="81" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
-        <v>217</v>
+        <v>73</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>229</v>
+        <v>74</v>
       </c>
       <c r="D81" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G81" s="16"/>
       <c r="L81" s="16"/>
       <c r="M81"/>
     </row>
-    <row r="82" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" s="16"/>
+      <c r="L82" s="17"/>
+      <c r="M82"/>
+    </row>
+    <row r="83" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A83" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G82" s="16"/>
-      <c r="L82" s="16"/>
-      <c r="M82"/>
-    </row>
-    <row r="83" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D83" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F83" s="2" t="s">
+        <v>266</v>
+      </c>
       <c r="G83" s="16"/>
-      <c r="L83" s="17"/>
+      <c r="L83" s="16"/>
       <c r="M83"/>
     </row>
-    <row r="84" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
+    <row r="84" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>269</v>
+      <c r="D84" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>300</v>
       </c>
       <c r="G84" s="16"/>
       <c r="L84" s="16"/>
       <c r="M84"/>
     </row>
-    <row r="85" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>303</v>
+    <row r="85" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G85" s="16"/>
       <c r="L85" s="16"/>
       <c r="M85"/>
     </row>
-    <row r="86" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
+    <row r="86" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>19</v>
+      <c r="D86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>208</v>
       </c>
       <c r="G86" s="16"/>
       <c r="L86" s="16"/>
       <c r="M86"/>
     </row>
-    <row r="87" spans="1:13" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A87" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D87" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>211</v>
+    <row r="87" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="G87" s="16"/>
       <c r="L87" s="16"/>
@@ -3481,45 +3472,45 @@
     </row>
     <row r="88" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="G88" s="16"/>
       <c r="L88" s="16"/>
       <c r="M88"/>
     </row>
-    <row r="89" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" s="2" t="s">
+    <row r="89" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A89" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D89" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="G89" s="16"/>
       <c r="L89" s="16"/>
@@ -3527,165 +3518,165 @@
     </row>
     <row r="90" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A90" s="7" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="D90" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E90" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="G90" s="16"/>
       <c r="L90" s="16"/>
       <c r="M90"/>
     </row>
     <row r="91" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D91" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F91" s="7" t="s">
+      <c r="A91" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="D91" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G91" s="16"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="21"/>
+      <c r="I91" s="21"/>
+      <c r="J91" s="21"/>
+      <c r="K91" s="21" t="s">
+        <v>4</v>
+      </c>
       <c r="L91" s="16"/>
       <c r="M91"/>
     </row>
-    <row r="92" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="21" t="s">
-        <v>312</v>
-      </c>
-      <c r="B92" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="21" t="s">
-        <v>313</v>
-      </c>
-      <c r="D92" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="22"/>
-      <c r="H92" s="21"/>
-      <c r="I92" s="21"/>
-      <c r="J92" s="21"/>
-      <c r="K92" s="21" t="s">
-        <v>4</v>
-      </c>
+    <row r="92" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G92" s="16"/>
       <c r="L92" s="16"/>
       <c r="M92"/>
     </row>
-    <row r="93" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
       <c r="D93" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E93" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="G93" s="16"/>
+      <c r="J93" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L93" s="16"/>
       <c r="M93"/>
     </row>
     <row r="94" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
+        <v>147</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="D94" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G94" s="16"/>
-      <c r="J94" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L94" s="16"/>
       <c r="M94"/>
     </row>
     <row r="95" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>151</v>
+        <v>96</v>
       </c>
       <c r="D95" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>4</v>
+        <v>264</v>
       </c>
       <c r="G95" s="16"/>
       <c r="L95" s="16"/>
       <c r="M95"/>
     </row>
-    <row r="96" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>98</v>
+        <v>197</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>10</v>
+        <v>198</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>99</v>
+        <v>199</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="G96" s="16"/>
       <c r="L96" s="16"/>
@@ -3693,13 +3684,13 @@
     </row>
     <row r="97" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>200</v>
+        <v>298</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>201</v>
+        <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>202</v>
+        <v>299</v>
       </c>
       <c r="D97" s="2" t="b">
         <v>0</v>
@@ -3708,21 +3699,24 @@
         <v>1</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>251</v>
+        <v>4</v>
       </c>
       <c r="G97" s="16"/>
+      <c r="H97" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="L97" s="16"/>
       <c r="M97"/>
     </row>
     <row r="98" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>301</v>
+        <v>244</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>5</v>
+        <v>245</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>302</v>
+        <v>246</v>
       </c>
       <c r="D98" s="2" t="b">
         <v>0</v>
@@ -3730,144 +3724,138 @@
       <c r="E98" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F98" s="2" t="s">
-        <v>4</v>
+      <c r="F98" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="G98" s="16"/>
-      <c r="H98" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="L98" s="16"/>
       <c r="M98"/>
     </row>
-    <row r="99" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>249</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
       <c r="D99" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F99" s="6" t="s">
-        <v>250</v>
+      <c r="F99" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="G99" s="16"/>
       <c r="L99" s="16"/>
       <c r="M99"/>
     </row>
-    <row r="100" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="D100" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="2" t="b">
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>303</v>
+        <v>16</v>
       </c>
       <c r="G100" s="16"/>
       <c r="L100" s="16"/>
       <c r="M100"/>
     </row>
-    <row r="101" spans="1:13" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>16</v>
+    <row r="101" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" t="s">
+        <v>271</v>
+      </c>
+      <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" t="s">
+        <v>272</v>
+      </c>
+      <c r="D101" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" t="s">
+        <v>300</v>
       </c>
       <c r="G101" s="16"/>
       <c r="L101" s="16"/>
-      <c r="M101"/>
-    </row>
-    <row r="102" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" t="s">
-        <v>274</v>
-      </c>
-      <c r="B102" t="s">
-        <v>10</v>
-      </c>
-      <c r="C102" t="s">
-        <v>275</v>
-      </c>
-      <c r="D102" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" t="b">
-        <v>1</v>
-      </c>
-      <c r="F102" t="s">
-        <v>303</v>
+    </row>
+    <row r="102" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="G102" s="16"/>
       <c r="L102" s="16"/>
+      <c r="M102"/>
     </row>
     <row r="103" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="D103" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F103" s="6" t="s">
-        <v>288</v>
+      <c r="F103" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G103" s="16"/>
       <c r="L103" s="16"/>
       <c r="M103"/>
     </row>
-    <row r="104" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>105</v>
+        <v>201</v>
       </c>
       <c r="D104" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E104" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G104" s="16"/>
       <c r="L104" s="16"/>
@@ -3875,77 +3863,80 @@
     </row>
     <row r="105" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>203</v>
+        <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>204</v>
+        <v>106</v>
       </c>
       <c r="D105" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="G105" s="16"/>
       <c r="L105" s="16"/>
       <c r="M105"/>
     </row>
-    <row r="106" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="D106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" s="16"/>
+      <c r="L106" s="17"/>
+      <c r="M106"/>
+    </row>
+    <row r="107" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A107" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D106" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G106" s="16"/>
-      <c r="L106" s="16"/>
-      <c r="M106"/>
-    </row>
-    <row r="107" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
+      <c r="B107" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>0</v>
+      <c r="D107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="G107" s="16"/>
-      <c r="L107" s="17"/>
+      <c r="L107" s="16"/>
       <c r="M107"/>
     </row>
     <row r="108" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C108" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B108" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>113</v>
-      </c>
       <c r="D108" s="7" t="b">
         <v>1</v>
       </c>
@@ -3953,7 +3944,7 @@
         <v>0</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G108" s="16"/>
       <c r="L108" s="16"/>
@@ -3961,45 +3952,45 @@
     </row>
     <row r="109" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B109" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="D109" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E109" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>218</v>
+        <v>16</v>
       </c>
       <c r="G109" s="16"/>
       <c r="L109" s="16"/>
       <c r="M109"/>
     </row>
-    <row r="110" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="7" t="s">
+    <row r="110" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B110" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D110" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="7" t="s">
-        <v>16</v>
+      <c r="D110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G110" s="16"/>
       <c r="L110" s="16"/>
@@ -4007,16 +3998,16 @@
     </row>
     <row r="111" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="D111" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" s="2" t="b">
         <v>1</v>
@@ -4030,16 +4021,16 @@
     </row>
     <row r="112" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="D112" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112" s="2" t="b">
         <v>1</v>
@@ -4048,18 +4039,21 @@
         <v>4</v>
       </c>
       <c r="G112" s="16"/>
+      <c r="H112" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="L112" s="16"/>
       <c r="M112"/>
     </row>
-    <row r="113" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="D113" s="2" t="b">
         <v>0</v>
@@ -4071,29 +4065,30 @@
         <v>4</v>
       </c>
       <c r="G113" s="16"/>
-      <c r="H113" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="H113"/>
+      <c r="I113"/>
+      <c r="J113"/>
+      <c r="K113"/>
       <c r="L113" s="16"/>
       <c r="M113"/>
     </row>
-    <row r="114" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A114" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D114" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F114" s="2" t="s">
+    <row r="114" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
+        <v>273</v>
+      </c>
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" t="s">
+        <v>274</v>
+      </c>
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" t="s">
         <v>4</v>
       </c>
       <c r="G114" s="16"/>
@@ -4102,65 +4097,63 @@
       <c r="J114"/>
       <c r="K114"/>
       <c r="L114" s="16"/>
-      <c r="M114"/>
-    </row>
-    <row r="115" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" t="s">
-        <v>276</v>
-      </c>
-      <c r="B115" t="s">
-        <v>5</v>
-      </c>
-      <c r="C115" t="s">
-        <v>277</v>
-      </c>
-      <c r="D115" t="b">
-        <v>0</v>
-      </c>
-      <c r="E115" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" t="s">
+    </row>
+    <row r="115" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A115" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D115" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" s="16"/>
+      <c r="L115" s="16"/>
+    </row>
+    <row r="116" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D116" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G115" s="16"/>
-      <c r="H115"/>
-      <c r="I115"/>
-      <c r="J115"/>
-      <c r="K115"/>
-      <c r="L115" s="16"/>
-    </row>
-    <row r="116" spans="1:13" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A116" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B116" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D116" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F116" s="7" t="s">
+      <c r="G116" s="16"/>
+      <c r="H116" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G116" s="16"/>
       <c r="L116" s="16"/>
     </row>
     <row r="117" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D117" s="2" t="b">
         <v>1</v>
@@ -4179,113 +4172,91 @@
     </row>
     <row r="118" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D118" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E118" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>4</v>
+        <v>300</v>
       </c>
       <c r="G118" s="16"/>
-      <c r="H118" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="L118" s="16"/>
     </row>
     <row r="119" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
-        <v>130</v>
+        <v>286</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C119" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G119" s="16"/>
+      <c r="L119" s="17"/>
+    </row>
+    <row r="120" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A120" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D120" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G120" s="16"/>
+      <c r="L120" s="16"/>
+    </row>
+    <row r="121" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A121" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D119" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E119" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="G119" s="16"/>
-      <c r="L119" s="16"/>
-    </row>
-    <row r="120" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A120" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D120" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E120" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G120" s="16"/>
-      <c r="L120" s="17"/>
-    </row>
-    <row r="121" spans="1:13" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A121" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="D121" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E121" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="G121" s="16"/>
       <c r="L121" s="16"/>
     </row>
-    <row r="122" spans="1:13" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A122" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D122" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E122" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G122" s="16"/>
-      <c r="L122" s="16"/>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M122"/>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.4">
       <c r="M123"/>
@@ -4349,9 +4320,6 @@
     </row>
     <row r="143" spans="13:13" x14ac:dyDescent="0.4">
       <c r="M143"/>
-    </row>
-    <row r="144" spans="13:13" x14ac:dyDescent="0.4">
-      <c r="M144"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4359,10 +4327,10 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4389,48 +4357,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>